<commit_message>
AITATR3-51 Revisi sweeping equalignorecase + AITATR3-46 ganti nama TC TabJobData
</commit_message>
<xml_diff>
--- a/Excel/2. DataFile_NAP_CF4W.xlsx
+++ b/Excel/2. DataFile_NAP_CF4W.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="769" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="769" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="0.Setting" sheetId="5" r:id="rId1"/>
@@ -24683,9 +24683,6 @@
     <t>PERUSAHAAN TITAN</t>
   </si>
   <si>
-    <t>0002APP20211202485</t>
-  </si>
-  <si>
     <t>BLI</t>
   </si>
   <si>
@@ -24720,6 +24717,9 @@
   </si>
   <si>
     <t>1000;1000;1000;1000;1000;1000</t>
+  </si>
+  <si>
+    <t>0002APP20211202503</t>
   </si>
 </sst>
 </file>
@@ -25308,6 +25308,8 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -25347,8 +25349,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -27644,14 +27644,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="95" t="s">
+    <row r="2" spans="1:5" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="97" t="s">
         <v>3213</v>
       </c>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="99"/>
     </row>
     <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
@@ -27661,14 +27661,14 @@
         <v>221</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="98" t="s">
+    <row r="4" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="100" t="s">
         <v>119</v>
       </c>
-      <c r="B4" s="99"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="100"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="101"/>
+      <c r="D4" s="101"/>
+      <c r="E4" s="102"/>
     </row>
     <row r="5" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="60" t="s">
@@ -27717,14 +27717,14 @@
         <v>228</v>
       </c>
     </row>
-    <row r="12" spans="1:5" s="101" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="98" t="s">
+    <row r="12" spans="1:5" s="103" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="100" t="s">
         <v>109</v>
       </c>
-      <c r="B12" s="99"/>
-      <c r="C12" s="99"/>
-      <c r="D12" s="99"/>
-      <c r="E12" s="100"/>
+      <c r="B12" s="101"/>
+      <c r="C12" s="101"/>
+      <c r="D12" s="101"/>
+      <c r="E12" s="102"/>
     </row>
     <row r="13" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="60" t="s">
@@ -27779,14 +27779,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="95" t="s">
+    <row r="20" spans="1:5" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="97" t="s">
         <v>3214</v>
       </c>
-      <c r="B20" s="96"/>
-      <c r="C20" s="96"/>
-      <c r="D20" s="96"/>
-      <c r="E20" s="97"/>
+      <c r="B20" s="98"/>
+      <c r="C20" s="98"/>
+      <c r="D20" s="98"/>
+      <c r="E20" s="99"/>
     </row>
     <row r="21" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="65" t="s">
@@ -27812,14 +27812,14 @@
         <v>800000</v>
       </c>
     </row>
-    <row r="24" spans="1:5" s="105" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="102" t="s">
+    <row r="24" spans="1:5" s="107" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="104" t="s">
         <v>3215</v>
       </c>
-      <c r="B24" s="103"/>
-      <c r="C24" s="103"/>
-      <c r="D24" s="103"/>
-      <c r="E24" s="104"/>
+      <c r="B24" s="105"/>
+      <c r="C24" s="105"/>
+      <c r="D24" s="105"/>
+      <c r="E24" s="106"/>
     </row>
     <row r="25" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="60" t="s">
@@ -27829,14 +27829,14 @@
         <v>241</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="98" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="98" t="s">
+    <row r="26" spans="1:5" s="100" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="100" t="s">
         <v>242</v>
       </c>
-      <c r="B26" s="99"/>
-      <c r="C26" s="99"/>
-      <c r="D26" s="99"/>
-      <c r="E26" s="99"/>
+      <c r="B26" s="101"/>
+      <c r="C26" s="101"/>
+      <c r="D26" s="101"/>
+      <c r="E26" s="101"/>
     </row>
     <row r="27" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
@@ -27894,11 +27894,11 @@
         <v>173</v>
       </c>
     </row>
-    <row r="34" spans="1:2" s="93" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="93" t="s">
+    <row r="34" spans="1:2" s="95" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="95" t="s">
         <v>3216</v>
       </c>
-      <c r="B34" s="94"/>
+      <c r="B34" s="96"/>
     </row>
     <row r="35" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="19" t="s">
@@ -28041,8 +28041,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="86" t="s">
+    <row r="2" spans="1:5" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="88" t="s">
         <v>3217</v>
       </c>
     </row>
@@ -28098,8 +28098,8 @@
         <v>257</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="86" t="s">
+    <row r="8" spans="1:5" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="88" t="s">
         <v>3218</v>
       </c>
     </row>
@@ -28147,8 +28147,8 @@
         <v>2618</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="86" t="s">
+    <row r="13" spans="1:5" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="88" t="s">
         <v>3219</v>
       </c>
     </row>
@@ -28290,14 +28290,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="95" t="s">
+    <row r="2" spans="1:5" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="97" t="s">
         <v>3220</v>
       </c>
-      <c r="B2" s="96"/>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="97"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="99"/>
     </row>
     <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="66" t="s">
@@ -28335,14 +28335,14 @@
         <v>271</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="95" t="s">
+    <row r="10" spans="1:5" s="97" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="97" t="s">
         <v>3221</v>
       </c>
-      <c r="B10" s="96"/>
-      <c r="C10" s="96"/>
-      <c r="D10" s="96"/>
-      <c r="E10" s="96"/>
+      <c r="B10" s="98"/>
+      <c r="C10" s="98"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="98"/>
     </row>
     <row r="11" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="58" t="s">
@@ -28520,14 +28520,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="95" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="95" t="s">
+    <row r="33" spans="1:5" s="97" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="97" t="s">
         <v>3222</v>
       </c>
-      <c r="B33" s="96"/>
-      <c r="C33" s="96"/>
-      <c r="D33" s="96"/>
-      <c r="E33" s="96"/>
+      <c r="B33" s="98"/>
+      <c r="C33" s="98"/>
+      <c r="D33" s="98"/>
+      <c r="E33" s="98"/>
     </row>
     <row r="34" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
@@ -28797,7 +28797,7 @@
         <v>2584</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>3420</v>
+        <v>3419</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>3193</v>
@@ -28808,7 +28808,7 @@
         <v>2585</v>
       </c>
       <c r="B3" s="85" t="s">
-        <v>3421</v>
+        <v>3420</v>
       </c>
       <c r="C3" s="15"/>
     </row>
@@ -28838,7 +28838,7 @@
         <v>2589</v>
       </c>
       <c r="B7" s="81" t="s">
-        <v>3419</v>
+        <v>3418</v>
       </c>
       <c r="C7" s="15"/>
     </row>
@@ -28853,10 +28853,10 @@
       <c r="C9" s="16"/>
     </row>
     <row r="10" spans="1:5" s="26" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="106" t="s">
+      <c r="A10" s="108" t="s">
         <v>2620</v>
       </c>
-      <c r="B10" s="106"/>
+      <c r="B10" s="108"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -28987,9 +28987,9 @@
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B41" sqref="B41"/>
+      <selection pane="topRight" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29024,14 +29024,14 @@
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="108" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="93" t="s">
+    <row r="3" spans="1:5" s="110" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="95" t="s">
         <v>2609</v>
       </c>
-      <c r="B3" s="94"/>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="107"/>
+      <c r="B3" s="96"/>
+      <c r="C3" s="96"/>
+      <c r="D3" s="96"/>
+      <c r="E3" s="109"/>
     </row>
     <row r="4" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -29100,7 +29100,7 @@
         <v>2591</v>
       </c>
       <c r="B12" s="14">
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -29127,14 +29127,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="108" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="93" t="s">
+    <row r="16" spans="1:5" s="110" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="95" t="s">
         <v>2613</v>
       </c>
-      <c r="B16" s="94"/>
-      <c r="C16" s="94"/>
-      <c r="D16" s="94"/>
-      <c r="E16" s="107"/>
+      <c r="B16" s="96"/>
+      <c r="C16" s="96"/>
+      <c r="D16" s="96"/>
+      <c r="E16" s="109"/>
     </row>
     <row r="17" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
@@ -29161,7 +29161,7 @@
         <v>261</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>3422</v>
+        <v>3421</v>
       </c>
     </row>
     <row r="21" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -29177,7 +29177,7 @@
         <v>2611</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>3422</v>
+        <v>3421</v>
       </c>
     </row>
     <row r="23" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -29193,7 +29193,7 @@
         <v>2600</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>3422</v>
+        <v>3421</v>
       </c>
     </row>
     <row r="25" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -29209,7 +29209,7 @@
         <v>2591</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>3311</v>
+        <v>3421</v>
       </c>
     </row>
     <row r="27" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -29252,11 +29252,11 @@
         <v>3288</v>
       </c>
     </row>
-    <row r="32" spans="1:2" s="108" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="93" t="s">
+    <row r="32" spans="1:2" s="110" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="95" t="s">
         <v>2597</v>
       </c>
-      <c r="B32" s="94"/>
+      <c r="B32" s="96"/>
     </row>
     <row r="33" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
@@ -29335,10 +29335,10 @@
       <c r="B44" s="20"/>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="109" t="s">
+      <c r="A45" s="111" t="s">
         <v>2601</v>
       </c>
-      <c r="B45" s="110"/>
+      <c r="B45" s="112"/>
     </row>
     <row r="46" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A46" s="25" t="s">
@@ -29368,7 +29368,7 @@
       <formula>A$2="Amount"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6:XFD6 A8:XFD8 A10:XFD10 A12:XFD12 A14:XFD14 A20:XFD20 A22:XFD22 A24:XFD24 A26:XFD26 A28:XFD28 A30:XFD30 A35:XFD35 A37:XFD37 A39:XFD39 A41:XFD41">
+  <conditionalFormatting sqref="A6:XFD6 A8:XFD8 A10:XFD10 A12:XFD12 A14:XFD14 A20:XFD20 A22:XFD22 A24:XFD24 A28:XFD28 A30:XFD30 A35:XFD35 A37:XFD37 A39:XFD39 A41:XFD41 A26:XFD26">
     <cfRule type="expression" dxfId="60" priority="1">
       <formula>A$2="Percentage"</formula>
     </cfRule>
@@ -29377,7 +29377,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
       <formula1>"Amount,Percentage"</formula1>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30 B24 B28 B26 B22 B35 B37 B39 B41 B20">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B30 B24 B28 B20 B22 B35 B37 B39 B41 B26">
       <formula1>B$2="Amount"</formula1>
     </dataValidation>
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B31 B29 B27 B25 B23 B36 B38 B40 B42 B21">
@@ -39955,9 +39955,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B35" sqref="B35"/>
+      <selection pane="topRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -39999,7 +39999,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>3410</v>
+        <v>3422</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>2578</v>
@@ -40034,8 +40034,8 @@
         <v>2561</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="86" t="s">
+    <row r="5" spans="1:6" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="88" t="s">
         <v>3196</v>
       </c>
     </row>
@@ -40103,7 +40103,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>3411</v>
+        <v>3410</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>90</v>
@@ -40240,7 +40240,7 @@
         <v>51</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>3412</v>
+        <v>3411</v>
       </c>
       <c r="F20" s="19" t="s">
         <v>2555</v>
@@ -40250,15 +40250,15 @@
       <c r="A21" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="111" t="s">
-        <v>3413</v>
+      <c r="B21" s="86" t="s">
+        <v>3412</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>2556</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="86" t="s">
+    <row r="22" spans="1:6" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="88" t="s">
         <v>3197</v>
       </c>
     </row>
@@ -40349,8 +40349,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="86" t="s">
+    <row r="27" spans="1:6" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="88" t="s">
         <v>3198</v>
       </c>
     </row>
@@ -40359,7 +40359,7 @@
         <v>74</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>3414</v>
+        <v>3413</v>
       </c>
       <c r="F28" s="19" t="s">
         <v>2557</v>
@@ -40649,7 +40649,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CW44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
@@ -42061,110 +42061,110 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:101" s="90" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="87" t="s">
+    <row r="30" spans="1:101" s="92" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="89" t="s">
         <v>3197</v>
       </c>
-      <c r="B30" s="88"/>
-      <c r="C30" s="88"/>
-      <c r="D30" s="88"/>
-      <c r="E30" s="88"/>
-      <c r="F30" s="88"/>
-      <c r="G30" s="88"/>
-      <c r="H30" s="88"/>
-      <c r="I30" s="88"/>
-      <c r="J30" s="88"/>
-      <c r="K30" s="88"/>
-      <c r="L30" s="88"/>
-      <c r="M30" s="88"/>
-      <c r="N30" s="88"/>
-      <c r="O30" s="88"/>
-      <c r="P30" s="88"/>
-      <c r="Q30" s="88"/>
-      <c r="R30" s="88"/>
-      <c r="S30" s="88"/>
-      <c r="T30" s="88"/>
-      <c r="U30" s="88"/>
-      <c r="V30" s="88"/>
-      <c r="W30" s="88"/>
-      <c r="X30" s="88"/>
-      <c r="Y30" s="88"/>
-      <c r="Z30" s="88"/>
-      <c r="AA30" s="88"/>
-      <c r="AB30" s="88"/>
-      <c r="AC30" s="88"/>
-      <c r="AD30" s="88"/>
-      <c r="AE30" s="88"/>
-      <c r="AF30" s="88"/>
-      <c r="AG30" s="88"/>
-      <c r="AH30" s="88"/>
-      <c r="AI30" s="88"/>
-      <c r="AJ30" s="88"/>
-      <c r="AK30" s="88"/>
-      <c r="AL30" s="88"/>
-      <c r="AM30" s="88"/>
-      <c r="AN30" s="88"/>
-      <c r="AO30" s="88"/>
-      <c r="AP30" s="88"/>
-      <c r="AQ30" s="88"/>
-      <c r="AR30" s="88"/>
-      <c r="AS30" s="88"/>
-      <c r="AT30" s="88"/>
-      <c r="AU30" s="88"/>
-      <c r="AV30" s="88"/>
-      <c r="AW30" s="88"/>
-      <c r="AX30" s="88"/>
-      <c r="AY30" s="88"/>
-      <c r="AZ30" s="88"/>
-      <c r="BA30" s="88"/>
-      <c r="BB30" s="88"/>
-      <c r="BC30" s="88"/>
-      <c r="BD30" s="88"/>
-      <c r="BE30" s="88"/>
-      <c r="BF30" s="88"/>
-      <c r="BG30" s="88"/>
-      <c r="BH30" s="88"/>
-      <c r="BI30" s="88"/>
-      <c r="BJ30" s="88"/>
-      <c r="BK30" s="88"/>
-      <c r="BL30" s="88"/>
-      <c r="BM30" s="88"/>
-      <c r="BN30" s="88"/>
-      <c r="BO30" s="88"/>
-      <c r="BP30" s="88"/>
-      <c r="BQ30" s="88"/>
-      <c r="BR30" s="88"/>
-      <c r="BS30" s="88"/>
-      <c r="BT30" s="88"/>
-      <c r="BU30" s="88"/>
-      <c r="BV30" s="88"/>
-      <c r="BW30" s="88"/>
-      <c r="BX30" s="88"/>
-      <c r="BY30" s="88"/>
-      <c r="BZ30" s="88"/>
-      <c r="CA30" s="88"/>
-      <c r="CB30" s="88"/>
-      <c r="CC30" s="88"/>
-      <c r="CD30" s="88"/>
-      <c r="CE30" s="88"/>
-      <c r="CF30" s="88"/>
-      <c r="CG30" s="88"/>
-      <c r="CH30" s="88"/>
-      <c r="CI30" s="88"/>
-      <c r="CJ30" s="88"/>
-      <c r="CK30" s="88"/>
-      <c r="CL30" s="88"/>
-      <c r="CM30" s="88"/>
-      <c r="CN30" s="88"/>
-      <c r="CO30" s="88"/>
-      <c r="CP30" s="88"/>
-      <c r="CQ30" s="88"/>
-      <c r="CR30" s="88"/>
-      <c r="CS30" s="88"/>
-      <c r="CT30" s="88"/>
-      <c r="CU30" s="88"/>
-      <c r="CV30" s="88"/>
-      <c r="CW30" s="89"/>
+      <c r="B30" s="90"/>
+      <c r="C30" s="90"/>
+      <c r="D30" s="90"/>
+      <c r="E30" s="90"/>
+      <c r="F30" s="90"/>
+      <c r="G30" s="90"/>
+      <c r="H30" s="90"/>
+      <c r="I30" s="90"/>
+      <c r="J30" s="90"/>
+      <c r="K30" s="90"/>
+      <c r="L30" s="90"/>
+      <c r="M30" s="90"/>
+      <c r="N30" s="90"/>
+      <c r="O30" s="90"/>
+      <c r="P30" s="90"/>
+      <c r="Q30" s="90"/>
+      <c r="R30" s="90"/>
+      <c r="S30" s="90"/>
+      <c r="T30" s="90"/>
+      <c r="U30" s="90"/>
+      <c r="V30" s="90"/>
+      <c r="W30" s="90"/>
+      <c r="X30" s="90"/>
+      <c r="Y30" s="90"/>
+      <c r="Z30" s="90"/>
+      <c r="AA30" s="90"/>
+      <c r="AB30" s="90"/>
+      <c r="AC30" s="90"/>
+      <c r="AD30" s="90"/>
+      <c r="AE30" s="90"/>
+      <c r="AF30" s="90"/>
+      <c r="AG30" s="90"/>
+      <c r="AH30" s="90"/>
+      <c r="AI30" s="90"/>
+      <c r="AJ30" s="90"/>
+      <c r="AK30" s="90"/>
+      <c r="AL30" s="90"/>
+      <c r="AM30" s="90"/>
+      <c r="AN30" s="90"/>
+      <c r="AO30" s="90"/>
+      <c r="AP30" s="90"/>
+      <c r="AQ30" s="90"/>
+      <c r="AR30" s="90"/>
+      <c r="AS30" s="90"/>
+      <c r="AT30" s="90"/>
+      <c r="AU30" s="90"/>
+      <c r="AV30" s="90"/>
+      <c r="AW30" s="90"/>
+      <c r="AX30" s="90"/>
+      <c r="AY30" s="90"/>
+      <c r="AZ30" s="90"/>
+      <c r="BA30" s="90"/>
+      <c r="BB30" s="90"/>
+      <c r="BC30" s="90"/>
+      <c r="BD30" s="90"/>
+      <c r="BE30" s="90"/>
+      <c r="BF30" s="90"/>
+      <c r="BG30" s="90"/>
+      <c r="BH30" s="90"/>
+      <c r="BI30" s="90"/>
+      <c r="BJ30" s="90"/>
+      <c r="BK30" s="90"/>
+      <c r="BL30" s="90"/>
+      <c r="BM30" s="90"/>
+      <c r="BN30" s="90"/>
+      <c r="BO30" s="90"/>
+      <c r="BP30" s="90"/>
+      <c r="BQ30" s="90"/>
+      <c r="BR30" s="90"/>
+      <c r="BS30" s="90"/>
+      <c r="BT30" s="90"/>
+      <c r="BU30" s="90"/>
+      <c r="BV30" s="90"/>
+      <c r="BW30" s="90"/>
+      <c r="BX30" s="90"/>
+      <c r="BY30" s="90"/>
+      <c r="BZ30" s="90"/>
+      <c r="CA30" s="90"/>
+      <c r="CB30" s="90"/>
+      <c r="CC30" s="90"/>
+      <c r="CD30" s="90"/>
+      <c r="CE30" s="90"/>
+      <c r="CF30" s="90"/>
+      <c r="CG30" s="90"/>
+      <c r="CH30" s="90"/>
+      <c r="CI30" s="90"/>
+      <c r="CJ30" s="90"/>
+      <c r="CK30" s="90"/>
+      <c r="CL30" s="90"/>
+      <c r="CM30" s="90"/>
+      <c r="CN30" s="90"/>
+      <c r="CO30" s="90"/>
+      <c r="CP30" s="90"/>
+      <c r="CQ30" s="90"/>
+      <c r="CR30" s="90"/>
+      <c r="CS30" s="90"/>
+      <c r="CT30" s="90"/>
+      <c r="CU30" s="90"/>
+      <c r="CV30" s="90"/>
+      <c r="CW30" s="91"/>
     </row>
     <row r="31" spans="1:101" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="62" t="s">
@@ -42253,110 +42253,110 @@
         <v>415</v>
       </c>
     </row>
-    <row r="35" spans="1:101" s="87" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="87" t="s">
+    <row r="35" spans="1:101" s="89" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="89" t="s">
         <v>3198</v>
       </c>
-      <c r="B35" s="88"/>
-      <c r="C35" s="88"/>
-      <c r="D35" s="88"/>
-      <c r="E35" s="88"/>
-      <c r="F35" s="88"/>
-      <c r="G35" s="88"/>
-      <c r="H35" s="88"/>
-      <c r="I35" s="88"/>
-      <c r="J35" s="88"/>
-      <c r="K35" s="88"/>
-      <c r="L35" s="88"/>
-      <c r="M35" s="88"/>
-      <c r="N35" s="88"/>
-      <c r="O35" s="88"/>
-      <c r="P35" s="88"/>
-      <c r="Q35" s="88"/>
-      <c r="R35" s="88"/>
-      <c r="S35" s="88"/>
-      <c r="T35" s="88"/>
-      <c r="U35" s="88"/>
-      <c r="V35" s="88"/>
-      <c r="W35" s="88"/>
-      <c r="X35" s="88"/>
-      <c r="Y35" s="88"/>
-      <c r="Z35" s="88"/>
-      <c r="AA35" s="88"/>
-      <c r="AB35" s="88"/>
-      <c r="AC35" s="88"/>
-      <c r="AD35" s="88"/>
-      <c r="AE35" s="88"/>
-      <c r="AF35" s="88"/>
-      <c r="AG35" s="88"/>
-      <c r="AH35" s="88"/>
-      <c r="AI35" s="88"/>
-      <c r="AJ35" s="88"/>
-      <c r="AK35" s="88"/>
-      <c r="AL35" s="88"/>
-      <c r="AM35" s="88"/>
-      <c r="AN35" s="88"/>
-      <c r="AO35" s="88"/>
-      <c r="AP35" s="88"/>
-      <c r="AQ35" s="88"/>
-      <c r="AR35" s="88"/>
-      <c r="AS35" s="88"/>
-      <c r="AT35" s="88"/>
-      <c r="AU35" s="88"/>
-      <c r="AV35" s="88"/>
-      <c r="AW35" s="88"/>
-      <c r="AX35" s="88"/>
-      <c r="AY35" s="88"/>
-      <c r="AZ35" s="88"/>
-      <c r="BA35" s="88"/>
-      <c r="BB35" s="88"/>
-      <c r="BC35" s="88"/>
-      <c r="BD35" s="88"/>
-      <c r="BE35" s="88"/>
-      <c r="BF35" s="88"/>
-      <c r="BG35" s="88"/>
-      <c r="BH35" s="88"/>
-      <c r="BI35" s="88"/>
-      <c r="BJ35" s="88"/>
-      <c r="BK35" s="88"/>
-      <c r="BL35" s="88"/>
-      <c r="BM35" s="88"/>
-      <c r="BN35" s="88"/>
-      <c r="BO35" s="88"/>
-      <c r="BP35" s="88"/>
-      <c r="BQ35" s="88"/>
-      <c r="BR35" s="88"/>
-      <c r="BS35" s="88"/>
-      <c r="BT35" s="88"/>
-      <c r="BU35" s="88"/>
-      <c r="BV35" s="88"/>
-      <c r="BW35" s="88"/>
-      <c r="BX35" s="88"/>
-      <c r="BY35" s="88"/>
-      <c r="BZ35" s="88"/>
-      <c r="CA35" s="88"/>
-      <c r="CB35" s="88"/>
-      <c r="CC35" s="88"/>
-      <c r="CD35" s="88"/>
-      <c r="CE35" s="88"/>
-      <c r="CF35" s="88"/>
-      <c r="CG35" s="88"/>
-      <c r="CH35" s="88"/>
-      <c r="CI35" s="88"/>
-      <c r="CJ35" s="88"/>
-      <c r="CK35" s="88"/>
-      <c r="CL35" s="88"/>
-      <c r="CM35" s="88"/>
-      <c r="CN35" s="88"/>
-      <c r="CO35" s="88"/>
-      <c r="CP35" s="88"/>
-      <c r="CQ35" s="88"/>
-      <c r="CR35" s="88"/>
-      <c r="CS35" s="88"/>
-      <c r="CT35" s="88"/>
-      <c r="CU35" s="88"/>
-      <c r="CV35" s="88"/>
-      <c r="CW35" s="88"/>
+      <c r="B35" s="90"/>
+      <c r="C35" s="90"/>
+      <c r="D35" s="90"/>
+      <c r="E35" s="90"/>
+      <c r="F35" s="90"/>
+      <c r="G35" s="90"/>
+      <c r="H35" s="90"/>
+      <c r="I35" s="90"/>
+      <c r="J35" s="90"/>
+      <c r="K35" s="90"/>
+      <c r="L35" s="90"/>
+      <c r="M35" s="90"/>
+      <c r="N35" s="90"/>
+      <c r="O35" s="90"/>
+      <c r="P35" s="90"/>
+      <c r="Q35" s="90"/>
+      <c r="R35" s="90"/>
+      <c r="S35" s="90"/>
+      <c r="T35" s="90"/>
+      <c r="U35" s="90"/>
+      <c r="V35" s="90"/>
+      <c r="W35" s="90"/>
+      <c r="X35" s="90"/>
+      <c r="Y35" s="90"/>
+      <c r="Z35" s="90"/>
+      <c r="AA35" s="90"/>
+      <c r="AB35" s="90"/>
+      <c r="AC35" s="90"/>
+      <c r="AD35" s="90"/>
+      <c r="AE35" s="90"/>
+      <c r="AF35" s="90"/>
+      <c r="AG35" s="90"/>
+      <c r="AH35" s="90"/>
+      <c r="AI35" s="90"/>
+      <c r="AJ35" s="90"/>
+      <c r="AK35" s="90"/>
+      <c r="AL35" s="90"/>
+      <c r="AM35" s="90"/>
+      <c r="AN35" s="90"/>
+      <c r="AO35" s="90"/>
+      <c r="AP35" s="90"/>
+      <c r="AQ35" s="90"/>
+      <c r="AR35" s="90"/>
+      <c r="AS35" s="90"/>
+      <c r="AT35" s="90"/>
+      <c r="AU35" s="90"/>
+      <c r="AV35" s="90"/>
+      <c r="AW35" s="90"/>
+      <c r="AX35" s="90"/>
+      <c r="AY35" s="90"/>
+      <c r="AZ35" s="90"/>
+      <c r="BA35" s="90"/>
+      <c r="BB35" s="90"/>
+      <c r="BC35" s="90"/>
+      <c r="BD35" s="90"/>
+      <c r="BE35" s="90"/>
+      <c r="BF35" s="90"/>
+      <c r="BG35" s="90"/>
+      <c r="BH35" s="90"/>
+      <c r="BI35" s="90"/>
+      <c r="BJ35" s="90"/>
+      <c r="BK35" s="90"/>
+      <c r="BL35" s="90"/>
+      <c r="BM35" s="90"/>
+      <c r="BN35" s="90"/>
+      <c r="BO35" s="90"/>
+      <c r="BP35" s="90"/>
+      <c r="BQ35" s="90"/>
+      <c r="BR35" s="90"/>
+      <c r="BS35" s="90"/>
+      <c r="BT35" s="90"/>
+      <c r="BU35" s="90"/>
+      <c r="BV35" s="90"/>
+      <c r="BW35" s="90"/>
+      <c r="BX35" s="90"/>
+      <c r="BY35" s="90"/>
+      <c r="BZ35" s="90"/>
+      <c r="CA35" s="90"/>
+      <c r="CB35" s="90"/>
+      <c r="CC35" s="90"/>
+      <c r="CD35" s="90"/>
+      <c r="CE35" s="90"/>
+      <c r="CF35" s="90"/>
+      <c r="CG35" s="90"/>
+      <c r="CH35" s="90"/>
+      <c r="CI35" s="90"/>
+      <c r="CJ35" s="90"/>
+      <c r="CK35" s="90"/>
+      <c r="CL35" s="90"/>
+      <c r="CM35" s="90"/>
+      <c r="CN35" s="90"/>
+      <c r="CO35" s="90"/>
+      <c r="CP35" s="90"/>
+      <c r="CQ35" s="90"/>
+      <c r="CR35" s="90"/>
+      <c r="CS35" s="90"/>
+      <c r="CT35" s="90"/>
+      <c r="CU35" s="90"/>
+      <c r="CV35" s="90"/>
+      <c r="CW35" s="90"/>
     </row>
     <row r="36" spans="1:101" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="58" t="s">
@@ -43145,8 +43145,8 @@
         <v>2561</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="86" t="s">
+    <row r="4" spans="1:6" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="88" t="s">
         <v>3201</v>
       </c>
     </row>
@@ -43453,8 +43453,8 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="86" t="s">
+    <row r="22" spans="1:6" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="88" t="s">
         <v>3197</v>
       </c>
     </row>
@@ -43539,8 +43539,8 @@
         <v>342</v>
       </c>
     </row>
-    <row r="27" spans="1:6" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="86" t="s">
+    <row r="27" spans="1:6" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="88" t="s">
         <v>3198</v>
       </c>
     </row>
@@ -43910,8 +43910,8 @@
         <v>2560</v>
       </c>
     </row>
-    <row r="4" spans="1:6" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="86" t="s">
+    <row r="4" spans="1:6" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="88" t="s">
         <v>3201</v>
       </c>
     </row>
@@ -44045,8 +44045,8 @@
         <v>115</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="86" t="s">
+    <row r="12" spans="1:6" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="88" t="s">
         <v>3198</v>
       </c>
     </row>
@@ -44602,8 +44602,8 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="86" t="s">
+    <row r="2" spans="1:5" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="88" t="s">
         <v>3202</v>
       </c>
     </row>
@@ -44633,8 +44633,8 @@
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="86" t="s">
+    <row r="7" spans="1:5" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="88" t="s">
         <v>3203</v>
       </c>
     </row>
@@ -44728,8 +44728,8 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:2" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="86" t="s">
+    <row r="20" spans="1:2" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="88" t="s">
         <v>3204</v>
       </c>
     </row>
@@ -44855,8 +44855,8 @@
         <v>163</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="86" t="s">
+    <row r="40" spans="1:2" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="88" t="s">
         <v>3205</v>
       </c>
     </row>
@@ -44898,8 +44898,8 @@
         <v>2427</v>
       </c>
     </row>
-    <row r="46" spans="1:2" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="86" t="s">
+    <row r="46" spans="1:2" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="88" t="s">
         <v>3206</v>
       </c>
     </row>
@@ -45113,14 +45113,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="91" t="s">
+    <row r="2" spans="1:5" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="93" t="s">
         <v>3207</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
+      <c r="B2" s="94"/>
+      <c r="C2" s="94"/>
+      <c r="D2" s="94"/>
+      <c r="E2" s="94"/>
     </row>
     <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
@@ -45152,14 +45152,14 @@
         <v>3304</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="91" t="s">
+    <row r="7" spans="1:5" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="93" t="s">
         <v>3208</v>
       </c>
-      <c r="B7" s="92"/>
-      <c r="C7" s="92"/>
-      <c r="D7" s="92"/>
-      <c r="E7" s="92"/>
+      <c r="B7" s="94"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="94"/>
     </row>
     <row r="8" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="59" t="s">
@@ -45190,7 +45190,7 @@
         <v>186</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>3415</v>
+        <v>3414</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -45198,15 +45198,15 @@
         <v>187</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>3416</v>
+        <v>3415</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>188</v>
       </c>
-      <c r="B13" s="112" t="s">
-        <v>3417</v>
+      <c r="B13" s="87" t="s">
+        <v>3416</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -45276,7 +45276,7 @@
         <v>198</v>
       </c>
       <c r="B22" s="84" t="s">
-        <v>3418</v>
+        <v>3417</v>
       </c>
     </row>
     <row r="23" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -45293,11 +45293,11 @@
       </c>
       <c r="B24" s="7"/>
     </row>
-    <row r="25" spans="1:2" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="91" t="s">
+    <row r="25" spans="1:2" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="93" t="s">
         <v>3209</v>
       </c>
-      <c r="B25" s="92"/>
+      <c r="B25" s="94"/>
     </row>
     <row r="26" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="59" t="s">
@@ -45307,11 +45307,11 @@
         <v>3305</v>
       </c>
     </row>
-    <row r="27" spans="1:2" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="91" t="s">
+    <row r="27" spans="1:2" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="93" t="s">
         <v>3210</v>
       </c>
-      <c r="B27" s="92"/>
+      <c r="B27" s="94"/>
     </row>
     <row r="28" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13" t="s">
@@ -45337,11 +45337,11 @@
         <v>417</v>
       </c>
     </row>
-    <row r="31" spans="1:2" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="91" t="s">
+    <row r="31" spans="1:2" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="93" t="s">
         <v>3211</v>
       </c>
-      <c r="B31" s="92"/>
+      <c r="B31" s="94"/>
     </row>
     <row r="32" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
@@ -45493,11 +45493,11 @@
         <v>3403</v>
       </c>
     </row>
-    <row r="51" spans="1:8" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="91" t="s">
+    <row r="51" spans="1:8" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="93" t="s">
         <v>3212</v>
       </c>
-      <c r="B51" s="92"/>
+      <c r="B51" s="94"/>
     </row>
     <row r="52" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="58" t="s">
@@ -45571,11 +45571,11 @@
         <v>3403</v>
       </c>
     </row>
-    <row r="61" spans="1:8" s="86" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="91" t="s">
+    <row r="61" spans="1:8" s="88" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="93" t="s">
         <v>3328</v>
       </c>
-      <c r="B61" s="92"/>
+      <c r="B61" s="94"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="82" t="s">

</xml_diff>

<commit_message>
AITATR3-57 Tab Financial Verify Advance / Arrear
</commit_message>
<xml_diff>
--- a/Excel/2. DataFile_NAP_CF4W.xlsx
+++ b/Excel/2. DataFile_NAP_CF4W.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="769" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" tabRatio="769" firstSheet="8" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="0.Setting" sheetId="5" r:id="rId1"/>
@@ -14444,7 +14444,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4217" uniqueCount="3423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4217" uniqueCount="3424">
   <si>
     <t>Count</t>
   </si>
@@ -24704,9 +24704,6 @@
     <t>BANDUNG, KOTA.</t>
   </si>
   <si>
-    <t>BP1010RFO</t>
-  </si>
-  <si>
     <t>PAJAK BUMI DAN BANGUNAN;REKENING LISTRIK;KARTU KELUARGA</t>
   </si>
   <si>
@@ -24720,6 +24717,12 @@
   </si>
   <si>
     <t>0002APP20211202503</t>
+  </si>
+  <si>
+    <t>Used</t>
+  </si>
+  <si>
+    <t>KB1010RFO</t>
   </si>
 </sst>
 </file>
@@ -27613,7 +27616,7 @@
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
       <selection pane="topRight" activeCell="B35" sqref="B35"/>
@@ -28012,7 +28015,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B5" sqref="B5"/>
+      <selection pane="topRight" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28084,7 +28087,7 @@
         <v>256</v>
       </c>
       <c r="B6" s="38">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="C6" s="38" t="s">
         <v>3242</v>
@@ -28261,8 +28264,8 @@
   <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28797,7 +28800,7 @@
         <v>2584</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>3419</v>
+        <v>3418</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>3193</v>
@@ -28808,7 +28811,7 @@
         <v>2585</v>
       </c>
       <c r="B3" s="85" t="s">
-        <v>3420</v>
+        <v>3419</v>
       </c>
       <c r="C3" s="15"/>
     </row>
@@ -28838,7 +28841,7 @@
         <v>2589</v>
       </c>
       <c r="B7" s="81" t="s">
-        <v>3418</v>
+        <v>3417</v>
       </c>
       <c r="C7" s="15"/>
     </row>
@@ -29161,7 +29164,7 @@
         <v>261</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>3421</v>
+        <v>3420</v>
       </c>
     </row>
     <row r="21" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -29177,7 +29180,7 @@
         <v>2611</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>3421</v>
+        <v>3420</v>
       </c>
     </row>
     <row r="23" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -29193,7 +29196,7 @@
         <v>2600</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>3421</v>
+        <v>3420</v>
       </c>
     </row>
     <row r="25" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -29209,7 +29212,7 @@
         <v>2591</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>3421</v>
+        <v>3420</v>
       </c>
     </row>
     <row r="27" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -39955,7 +39958,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B3" sqref="B3"/>
     </sheetView>
@@ -39999,7 +40002,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>3422</v>
+        <v>3421</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>2578</v>
@@ -40649,7 +40652,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CW44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
@@ -45083,10 +45086,10 @@
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A43" sqref="A43"/>
-      <selection pane="topRight" activeCell="B35" sqref="B35"/>
+      <selection pane="topRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45101,7 +45104,7 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>3276</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>24</v>
@@ -45174,7 +45177,7 @@
         <v>184</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>3389</v>
+        <v>3422</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -45214,7 +45217,7 @@
         <v>189</v>
       </c>
       <c r="B14" s="74">
-        <v>44734</v>
+        <v>44369</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -45260,7 +45263,7 @@
         <v>196</v>
       </c>
       <c r="B20" s="84">
-        <v>123198402</v>
+        <v>75346</v>
       </c>
     </row>
     <row r="21" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -45268,7 +45271,7 @@
         <v>197</v>
       </c>
       <c r="B21" s="84">
-        <v>102983202</v>
+        <v>82364</v>
       </c>
     </row>
     <row r="22" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -45276,7 +45279,7 @@
         <v>198</v>
       </c>
       <c r="B22" s="84" t="s">
-        <v>3417</v>
+        <v>3423</v>
       </c>
     </row>
     <row r="23" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -45284,7 +45287,7 @@
         <v>3280</v>
       </c>
       <c r="B23" s="84">
-        <v>12392</v>
+        <v>527245</v>
       </c>
     </row>
     <row r="24" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -45582,7 +45585,7 @@
         <v>3329</v>
       </c>
       <c r="B62" s="39" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="C62" s="18"/>
       <c r="D62" s="18"/>

</xml_diff>

<commit_message>
AITATR3-54 Dupcheck - Checking Flow Dupcheck
</commit_message>
<xml_diff>
--- a/Excel/2. DataFile_NAP_CF4W.xlsx
+++ b/Excel/2. DataFile_NAP_CF4W.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="5" firstSheet="2" tabRatio="769" windowHeight="7650" windowWidth="20490" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" tabRatio="769" windowHeight="7650" windowWidth="20490" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="0.Setting" r:id="rId1" sheetId="5"/>
@@ -14444,7 +14444,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4252" uniqueCount="3433">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4219" uniqueCount="3430">
   <si>
     <t>Count</t>
   </si>
@@ -24731,25 +24731,16 @@
     <t>2193213821638612</t>
   </si>
   <si>
-    <t>0002APP20211202566</t>
-  </si>
-  <si>
     <t>New;New;New</t>
   </si>
   <si>
     <t>FT Joy;Ft SANI;ft andri;ft Commissioner andi;ft bod;FT EMP</t>
   </si>
   <si>
-    <t>0002APP20211202570</t>
-  </si>
-  <si>
-    <t>0002APP20211202571</t>
-  </si>
-  <si>
-    <t>0002APP20211202573</t>
-  </si>
-  <si>
     <t>0002APP20211202575</t>
+  </si>
+  <si>
+    <t>0002APP20211202611</t>
   </si>
 </sst>
 </file>
@@ -39985,9 +39976,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
-      <selection activeCell="B15" pane="topRight" sqref="B15"/>
+      <selection activeCell="D16" pane="topRight" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40029,7 +40020,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>3432</v>
+        <v>3429</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>2577</v>
@@ -40122,7 +40113,7 @@
         <v>2549</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>3421</v>
+        <v>3229</v>
       </c>
       <c r="F9" s="19" t="s">
         <v>2550</v>
@@ -44299,7 +44290,7 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
       <selection activeCell="B7" pane="topRight" sqref="B7"/>
     </sheetView>
@@ -44366,7 +44357,7 @@
         <v>2574</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>3427</v>
+        <v>3426</v>
       </c>
     </row>
     <row customFormat="1" r="7" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -44374,7 +44365,7 @@
         <v>2575</v>
       </c>
       <c r="B7" s="83" t="s">
-        <v>3428</v>
+        <v>3427</v>
       </c>
     </row>
     <row customFormat="1" r="8" s="19" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AITATR3-56 NAP 4 - Enhance CDC x Dupcheck
</commit_message>
<xml_diff>
--- a/Excel/2. DataFile_NAP_CF4W.xlsx
+++ b/Excel/2. DataFile_NAP_CF4W.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="1" tabRatio="769" windowHeight="7650" windowWidth="20490" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="5" firstSheet="2" tabRatio="769" windowHeight="7650" windowWidth="20490" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="0.Setting" r:id="rId1" sheetId="5"/>
@@ -14444,7 +14444,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4219" uniqueCount="3430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4219" uniqueCount="3428">
   <si>
     <t>Count</t>
   </si>
@@ -24164,15 +24164,9 @@
     <t>2312313923920000</t>
   </si>
   <si>
-    <t>0002CUST20211204141</t>
-  </si>
-  <si>
     <t>0002CUST20211204148</t>
   </si>
   <si>
-    <t>FT COMPANY LOOP</t>
-  </si>
-  <si>
     <t>FT COMPANY CUSTMAIN</t>
   </si>
   <si>
@@ -24668,9 +24662,6 @@
     <t>ROSA</t>
   </si>
   <si>
-    <t>PERUSAHAAN TITAN</t>
-  </si>
-  <si>
     <t>BLI</t>
   </si>
   <si>
@@ -24713,12 +24704,6 @@
     <t>FT DAVID;Ft janu;ft HANDY</t>
   </si>
   <si>
-    <t>New;Select;New;Select;New;Select</t>
-  </si>
-  <si>
-    <t>FT RICKY</t>
-  </si>
-  <si>
     <t>1231233451299999</t>
   </si>
   <si>
@@ -24734,13 +24719,22 @@
     <t>New;New;New</t>
   </si>
   <si>
-    <t>FT Joy;Ft SANI;ft andri;ft Commissioner andi;ft bod;FT EMP</t>
-  </si>
-  <si>
-    <t>0002APP20211202575</t>
-  </si>
-  <si>
-    <t>0002APP20211202611</t>
+    <t>FT DAVID;FT JANU;FT HANDY</t>
+  </si>
+  <si>
+    <t>New;Select;Select;New;Select;Select</t>
+  </si>
+  <si>
+    <t>0002APP20211202718</t>
+  </si>
+  <si>
+    <t>null;FT SANI;DOGE BOTHER;FT BOD;FT EMP</t>
+  </si>
+  <si>
+    <t>ft joy;ft sani;FT ANDRI;ft chris;ft bod;ft emp</t>
+  </si>
+  <si>
+    <t>FT JOY;FT SANI;FT BOD;FT EMP</t>
   </si>
 </sst>
 </file>
@@ -27413,13 +27407,13 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>3275</v>
+        <v>3273</v>
       </c>
       <c r="D1" t="s">
-        <v>3275</v>
+        <v>3273</v>
       </c>
       <c r="E1" t="s">
-        <v>3275</v>
+        <v>3273</v>
       </c>
       <c r="F1" s="19" t="s">
         <v>24</v>
@@ -27428,7 +27422,7 @@
         <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>3275</v>
+        <v>3273</v>
       </c>
     </row>
     <row customFormat="1" r="2" s="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -27446,13 +27440,13 @@
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="19" t="s">
-        <v>3276</v>
+        <v>3274</v>
       </c>
       <c r="F3" s="7" t="s">
         <v>3190</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>3276</v>
+        <v>3274</v>
       </c>
       <c r="H3" s="7"/>
     </row>
@@ -27461,7 +27455,7 @@
         <v>180</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>3301</v>
+        <v>3299</v>
       </c>
       <c r="C4" s="8"/>
       <c r="E4" s="8" t="s">
@@ -27494,10 +27488,10 @@
         <v>216</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>3305</v>
+        <v>3303</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>3278</v>
+        <v>3276</v>
       </c>
       <c r="E6" s="9" t="s">
         <v>217</v>
@@ -27586,7 +27580,7 @@
         <v>190</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>3277</v>
+        <v>3275</v>
       </c>
     </row>
   </sheetData>
@@ -27696,7 +27690,7 @@
         <v>222</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>3402</v>
+        <v>3400</v>
       </c>
     </row>
     <row customFormat="1" r="6" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -28108,7 +28102,7 @@
         <v>0.3</v>
       </c>
       <c r="C6" s="38" t="s">
-        <v>3241</v>
+        <v>3239</v>
       </c>
     </row>
     <row customFormat="1" r="7" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -28595,7 +28589,7 @@
         <v>301</v>
       </c>
       <c r="B39" s="19" t="s">
-        <v>3256</v>
+        <v>3254</v>
       </c>
     </row>
   </sheetData>
@@ -28818,7 +28812,7 @@
         <v>2583</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>3414</v>
+        <v>3411</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>3192</v>
@@ -28829,7 +28823,7 @@
         <v>2584</v>
       </c>
       <c r="B3" s="85" t="s">
-        <v>3415</v>
+        <v>3412</v>
       </c>
       <c r="C3" s="15"/>
     </row>
@@ -28859,7 +28853,7 @@
         <v>2588</v>
       </c>
       <c r="B7" s="81" t="s">
-        <v>3413</v>
+        <v>3410</v>
       </c>
       <c r="C7" s="15"/>
     </row>
@@ -29174,7 +29168,7 @@
         <v>2631</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>3309</v>
+        <v>3307</v>
       </c>
     </row>
     <row customFormat="1" r="20" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -29182,7 +29176,7 @@
         <v>261</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>3416</v>
+        <v>3413</v>
       </c>
     </row>
     <row customFormat="1" r="21" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -29190,7 +29184,7 @@
         <v>2598</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>3284</v>
+        <v>3282</v>
       </c>
     </row>
     <row customFormat="1" r="22" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -29198,7 +29192,7 @@
         <v>2610</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>3416</v>
+        <v>3413</v>
       </c>
     </row>
     <row customFormat="1" r="23" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -29206,7 +29200,7 @@
         <v>2611</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>3285</v>
+        <v>3283</v>
       </c>
     </row>
     <row customFormat="1" r="24" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -29214,7 +29208,7 @@
         <v>2599</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>3416</v>
+        <v>3413</v>
       </c>
     </row>
     <row customFormat="1" r="25" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -29230,7 +29224,7 @@
         <v>2590</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>3416</v>
+        <v>3413</v>
       </c>
     </row>
     <row customFormat="1" r="27" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -29246,7 +29240,7 @@
         <v>2592</v>
       </c>
       <c r="B28" s="27" t="s">
-        <v>3310</v>
+        <v>3308</v>
       </c>
     </row>
     <row customFormat="1" r="29" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -29254,7 +29248,7 @@
         <v>2593</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>3286</v>
+        <v>3284</v>
       </c>
     </row>
     <row customFormat="1" r="30" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -29262,7 +29256,7 @@
         <v>2594</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>3310</v>
+        <v>3308</v>
       </c>
     </row>
     <row customFormat="1" r="31" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -29270,7 +29264,7 @@
         <v>2595</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>3287</v>
+        <v>3285</v>
       </c>
     </row>
     <row customFormat="1" r="32" s="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -29302,7 +29296,7 @@
         <v>2598</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>3288</v>
+        <v>3286</v>
       </c>
     </row>
     <row customFormat="1" r="37" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -29316,7 +29310,7 @@
         <v>2589</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>3289</v>
+        <v>3287</v>
       </c>
     </row>
     <row customFormat="1" r="39" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -29330,7 +29324,7 @@
         <v>2591</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>3290</v>
+        <v>3288</v>
       </c>
     </row>
     <row customFormat="1" r="41" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -29344,7 +29338,7 @@
         <v>2593</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>3291</v>
+        <v>3289</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -29516,7 +29510,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
-      <selection activeCell="B4" pane="topRight" sqref="B4"/>
+      <selection activeCell="B5" pane="topRight" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29556,8 +29550,8 @@
       <c r="A3" s="60" t="s">
         <v>119</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>3294</v>
+      <c r="B3" t="s">
+        <v>3229</v>
       </c>
     </row>
     <row customFormat="1" r="4" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -29572,8 +29566,8 @@
       <c r="A5" s="60" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="19" t="s">
-        <v>3404</v>
+      <c r="B5" t="s">
+        <v>3422</v>
       </c>
     </row>
     <row customFormat="1" r="6" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -29588,8 +29582,8 @@
       <c r="A7" s="60" t="s">
         <v>2581</v>
       </c>
-      <c r="B7" s="19" t="s">
-        <v>3405</v>
+      <c r="B7" t="s">
+        <v>3427</v>
       </c>
     </row>
     <row customFormat="1" r="8" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -29708,7 +29702,7 @@
   <sheetData>
     <row r="1" spans="1:118" x14ac:dyDescent="0.25">
       <c r="A1" s="30" t="s">
-        <v>3334</v>
+        <v>3332</v>
       </c>
       <c r="B1" s="30" t="s">
         <v>2632</v>
@@ -29720,7 +29714,7 @@
         <v>2635</v>
       </c>
       <c r="I1" s="30" t="s">
-        <v>3337</v>
+        <v>3335</v>
       </c>
       <c r="J1" s="30" t="s">
         <v>2632</v>
@@ -29861,34 +29855,34 @@
         <v>262</v>
       </c>
       <c r="CW1" s="30" t="s">
-        <v>3246</v>
+        <v>3244</v>
       </c>
       <c r="CY1" s="30" t="s">
         <v>267</v>
       </c>
       <c r="DA1" s="30" t="s">
-        <v>3255</v>
+        <v>3253</v>
       </c>
       <c r="DC1" s="30" t="s">
         <v>301</v>
       </c>
       <c r="DE1" s="57" t="s">
-        <v>3257</v>
+        <v>3255</v>
       </c>
       <c r="DG1" s="30" t="s">
-        <v>3335</v>
+        <v>3333</v>
       </c>
       <c r="DH1" s="30" t="s">
         <v>2632</v>
       </c>
       <c r="DJ1" s="30" t="s">
-        <v>3332</v>
+        <v>3330</v>
       </c>
       <c r="DK1" s="30" t="s">
         <v>2632</v>
       </c>
       <c r="DM1" s="30" t="s">
-        <v>3333</v>
+        <v>3331</v>
       </c>
       <c r="DN1" s="30" t="s">
         <v>2632</v>
@@ -29908,10 +29902,10 @@
         <v>318</v>
       </c>
       <c r="I2" s="30" t="s">
-        <v>3338</v>
+        <v>3336</v>
       </c>
       <c r="J2" s="30" t="s">
-        <v>3363</v>
+        <v>3361</v>
       </c>
       <c r="M2" s="30" t="s">
         <v>319</v>
@@ -30047,7 +30041,7 @@
         <v>263</v>
       </c>
       <c r="CW2" s="30" t="s">
-        <v>3247</v>
+        <v>3245</v>
       </c>
       <c r="CY2" s="30" t="s">
         <v>268</v>
@@ -30094,10 +30088,10 @@
         <v>339</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>3339</v>
+        <v>3337</v>
       </c>
       <c r="J3" s="30" t="s">
-        <v>3364</v>
+        <v>3362</v>
       </c>
       <c r="M3" s="30" t="s">
         <v>340</v>
@@ -30235,16 +30229,16 @@
         <v>221</v>
       </c>
       <c r="CW3" s="30" t="s">
+        <v>3246</v>
+      </c>
+      <c r="CY3" s="30" t="s">
         <v>3248</v>
       </c>
-      <c r="CY3" s="30" t="s">
-        <v>3250</v>
-      </c>
       <c r="DA3" s="30" t="s">
-        <v>3245</v>
+        <v>3243</v>
       </c>
       <c r="DC3" s="30" t="s">
-        <v>3256</v>
+        <v>3254</v>
       </c>
       <c r="DE3" s="32" t="s">
         <v>219</v>
@@ -30285,7 +30279,7 @@
         <v>368</v>
       </c>
       <c r="J4" s="30" t="s">
-        <v>3365</v>
+        <v>3363</v>
       </c>
       <c r="M4" s="30" t="s">
         <v>69</v>
@@ -30399,13 +30393,13 @@
         <v>537</v>
       </c>
       <c r="CU4" s="30" t="s">
-        <v>3242</v>
+        <v>3240</v>
       </c>
       <c r="CW4" s="30" t="s">
         <v>272</v>
       </c>
       <c r="CY4" s="30" t="s">
-        <v>3251</v>
+        <v>3249</v>
       </c>
       <c r="DG4" s="30" t="s">
         <v>408</v>
@@ -30443,7 +30437,7 @@
         <v>66</v>
       </c>
       <c r="J5" s="30" t="s">
-        <v>3357</v>
+        <v>3355</v>
       </c>
       <c r="M5" s="30" t="s">
         <v>392</v>
@@ -30539,13 +30533,13 @@
         <v>3193</v>
       </c>
       <c r="CU5" s="30" t="s">
-        <v>3243</v>
+        <v>3241</v>
       </c>
       <c r="CW5" s="30" t="s">
         <v>266</v>
       </c>
       <c r="CY5" s="30" t="s">
-        <v>3252</v>
+        <v>3250</v>
       </c>
       <c r="DG5" s="30" t="s">
         <v>543</v>
@@ -30661,10 +30655,10 @@
         <v>416</v>
       </c>
       <c r="CU6" s="30" t="s">
-        <v>3244</v>
+        <v>3242</v>
       </c>
       <c r="CW6" s="30" t="s">
-        <v>3249</v>
+        <v>3247</v>
       </c>
       <c r="CY6" s="30" t="s">
         <v>273</v>
@@ -30702,10 +30696,10 @@
         <v>428</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>3340</v>
+        <v>3338</v>
       </c>
       <c r="J7" s="30" t="s">
-        <v>3366</v>
+        <v>3364</v>
       </c>
       <c r="M7" s="30" t="s">
         <v>429</v>
@@ -30774,7 +30768,7 @@
         <v>3226</v>
       </c>
       <c r="CY7" s="30" t="s">
-        <v>3253</v>
+        <v>3251</v>
       </c>
       <c r="DG7" s="30" t="s">
         <v>644</v>
@@ -30803,10 +30797,10 @@
         <v>441</v>
       </c>
       <c r="I8" s="30" t="s">
-        <v>3341</v>
+        <v>3339</v>
       </c>
       <c r="J8" s="30" t="s">
-        <v>3367</v>
+        <v>3365</v>
       </c>
       <c r="M8" s="30" t="s">
         <v>442</v>
@@ -30872,7 +30866,7 @@
         <v>3227</v>
       </c>
       <c r="CY8" s="30" t="s">
-        <v>3254</v>
+        <v>3252</v>
       </c>
       <c r="DG8" s="30" t="s">
         <v>651</v>
@@ -30901,10 +30895,10 @@
         <v>452</v>
       </c>
       <c r="I9" s="30" t="s">
-        <v>3342</v>
+        <v>3340</v>
       </c>
       <c r="J9" s="30" t="s">
-        <v>3368</v>
+        <v>3366</v>
       </c>
       <c r="M9" s="30" t="s">
         <v>453</v>
@@ -30988,10 +30982,10 @@
         <v>466</v>
       </c>
       <c r="I10" s="30" t="s">
-        <v>3343</v>
+        <v>3341</v>
       </c>
       <c r="J10" s="30" t="s">
-        <v>3369</v>
+        <v>3367</v>
       </c>
       <c r="M10" s="30" t="s">
         <v>467</v>
@@ -31015,7 +31009,7 @@
         <v>2670</v>
       </c>
       <c r="AX10" s="30" t="s">
-        <v>3263</v>
+        <v>3261</v>
       </c>
       <c r="BB10" s="30" t="s">
         <v>3143</v>
@@ -31069,10 +31063,10 @@
         <v>477</v>
       </c>
       <c r="I11" s="30" t="s">
-        <v>3344</v>
+        <v>3342</v>
       </c>
       <c r="J11" s="30" t="s">
-        <v>3370</v>
+        <v>3368</v>
       </c>
       <c r="M11" s="30" t="s">
         <v>478</v>
@@ -31143,7 +31137,7 @@
         <v>488</v>
       </c>
       <c r="J12" s="30" t="s">
-        <v>3371</v>
+        <v>3369</v>
       </c>
       <c r="M12" s="30" t="s">
         <v>489</v>
@@ -31167,7 +31161,7 @@
         <v>2672</v>
       </c>
       <c r="AX12" s="30" t="s">
-        <v>3330</v>
+        <v>3328</v>
       </c>
       <c r="BB12" s="30" t="s">
         <v>3145</v>
@@ -31209,10 +31203,10 @@
         <v>498</v>
       </c>
       <c r="I13" s="30" t="s">
-        <v>3345</v>
+        <v>3343</v>
       </c>
       <c r="J13" s="30" t="s">
-        <v>3372</v>
+        <v>3370</v>
       </c>
       <c r="M13" s="30" t="s">
         <v>499</v>
@@ -31274,10 +31268,10 @@
         <v>508</v>
       </c>
       <c r="I14" s="30" t="s">
-        <v>3346</v>
+        <v>3344</v>
       </c>
       <c r="J14" s="30" t="s">
-        <v>3373</v>
+        <v>3371</v>
       </c>
       <c r="M14" s="30" t="s">
         <v>509</v>
@@ -31340,10 +31334,10 @@
         <v>518</v>
       </c>
       <c r="I15" s="30" t="s">
-        <v>3347</v>
+        <v>3345</v>
       </c>
       <c r="J15" s="30" t="s">
-        <v>3374</v>
+        <v>3372</v>
       </c>
       <c r="M15" s="30" t="s">
         <v>519</v>
@@ -31399,10 +31393,10 @@
         <v>527</v>
       </c>
       <c r="I16" s="30" t="s">
-        <v>3348</v>
+        <v>3346</v>
       </c>
       <c r="J16" s="30" t="s">
-        <v>3375</v>
+        <v>3373</v>
       </c>
       <c r="M16" s="30" t="s">
         <v>528</v>
@@ -31449,7 +31443,7 @@
         <v>536</v>
       </c>
       <c r="I17" s="30" t="s">
-        <v>3349</v>
+        <v>3347</v>
       </c>
       <c r="J17" s="30" t="s">
         <v>537</v>
@@ -31499,10 +31493,10 @@
         <v>546</v>
       </c>
       <c r="I18" s="30" t="s">
-        <v>3350</v>
+        <v>3348</v>
       </c>
       <c r="J18" s="30" t="s">
-        <v>3376</v>
+        <v>3374</v>
       </c>
       <c r="M18" s="30" t="s">
         <v>547</v>
@@ -31543,10 +31537,10 @@
         <v>555</v>
       </c>
       <c r="I19" s="30" t="s">
-        <v>3351</v>
+        <v>3349</v>
       </c>
       <c r="J19" s="30" t="s">
-        <v>3377</v>
+        <v>3375</v>
       </c>
       <c r="M19" s="30" t="s">
         <v>556</v>
@@ -31587,10 +31581,10 @@
         <v>564</v>
       </c>
       <c r="I20" s="30" t="s">
-        <v>3352</v>
+        <v>3350</v>
       </c>
       <c r="J20" s="30" t="s">
-        <v>3378</v>
+        <v>3376</v>
       </c>
       <c r="M20" s="30" t="s">
         <v>565</v>
@@ -31631,10 +31625,10 @@
         <v>573</v>
       </c>
       <c r="I21" s="30" t="s">
-        <v>3353</v>
+        <v>3351</v>
       </c>
       <c r="J21" s="30" t="s">
-        <v>3379</v>
+        <v>3377</v>
       </c>
       <c r="M21" s="30" t="s">
         <v>574</v>
@@ -31675,10 +31669,10 @@
         <v>582</v>
       </c>
       <c r="I22" s="30" t="s">
-        <v>3354</v>
+        <v>3352</v>
       </c>
       <c r="J22" s="30" t="s">
-        <v>3380</v>
+        <v>3378</v>
       </c>
       <c r="M22" s="30" t="s">
         <v>583</v>
@@ -31719,10 +31713,10 @@
         <v>590</v>
       </c>
       <c r="I23" s="30" t="s">
-        <v>3355</v>
+        <v>3353</v>
       </c>
       <c r="J23" s="30" t="s">
-        <v>3381</v>
+        <v>3379</v>
       </c>
       <c r="M23" s="30" t="s">
         <v>591</v>
@@ -31763,10 +31757,10 @@
         <v>598</v>
       </c>
       <c r="I24" s="30" t="s">
-        <v>3356</v>
+        <v>3354</v>
       </c>
       <c r="J24" s="30" t="s">
-        <v>3382</v>
+        <v>3380</v>
       </c>
       <c r="M24" s="30" t="s">
         <v>599</v>
@@ -31775,7 +31769,7 @@
         <v>600</v>
       </c>
       <c r="AN24" s="30" t="s">
-        <v>3264</v>
+        <v>3262</v>
       </c>
       <c r="AR24" s="30" t="s">
         <v>601</v>
@@ -31807,10 +31801,10 @@
         <v>605</v>
       </c>
       <c r="I25" s="30" t="s">
-        <v>3357</v>
+        <v>3355</v>
       </c>
       <c r="J25" s="30" t="s">
-        <v>3357</v>
+        <v>3355</v>
       </c>
       <c r="M25" s="30" t="s">
         <v>606</v>
@@ -31819,7 +31813,7 @@
         <v>607</v>
       </c>
       <c r="AN25" s="30" t="s">
-        <v>3265</v>
+        <v>3263</v>
       </c>
       <c r="AR25" s="30" t="s">
         <v>608</v>
@@ -31851,10 +31845,10 @@
         <v>612</v>
       </c>
       <c r="I26" s="30" t="s">
-        <v>3358</v>
+        <v>3356</v>
       </c>
       <c r="J26" s="30" t="s">
-        <v>3383</v>
+        <v>3381</v>
       </c>
       <c r="M26" s="30" t="s">
         <v>613</v>
@@ -31863,7 +31857,7 @@
         <v>614</v>
       </c>
       <c r="AN26" s="30" t="s">
-        <v>3266</v>
+        <v>3264</v>
       </c>
       <c r="AR26" s="30" t="s">
         <v>615</v>
@@ -31895,10 +31889,10 @@
         <v>619</v>
       </c>
       <c r="I27" s="30" t="s">
-        <v>3359</v>
+        <v>3357</v>
       </c>
       <c r="J27" s="30" t="s">
-        <v>3384</v>
+        <v>3382</v>
       </c>
       <c r="M27" s="30" t="s">
         <v>620</v>
@@ -31907,7 +31901,7 @@
         <v>621</v>
       </c>
       <c r="AN27" s="30" t="s">
-        <v>3267</v>
+        <v>3265</v>
       </c>
       <c r="AR27" s="30" t="s">
         <v>622</v>
@@ -31916,7 +31910,7 @@
         <v>2687</v>
       </c>
       <c r="CH27" s="30" t="s">
-        <v>3261</v>
+        <v>3259</v>
       </c>
       <c r="DG27" s="30" t="s">
         <v>1019</v>
@@ -31939,10 +31933,10 @@
         <v>626</v>
       </c>
       <c r="I28" s="30" t="s">
-        <v>3360</v>
+        <v>3358</v>
       </c>
       <c r="J28" s="30" t="s">
-        <v>3385</v>
+        <v>3383</v>
       </c>
       <c r="M28" s="30" t="s">
         <v>627</v>
@@ -31951,7 +31945,7 @@
         <v>628</v>
       </c>
       <c r="AN28" s="30" t="s">
-        <v>3268</v>
+        <v>3266</v>
       </c>
       <c r="AR28" s="30" t="s">
         <v>629</v>
@@ -31960,7 +31954,7 @@
         <v>2688</v>
       </c>
       <c r="CH28" s="30" t="s">
-        <v>3262</v>
+        <v>3260</v>
       </c>
       <c r="DG28" s="30" t="s">
         <v>1025</v>
@@ -31983,10 +31977,10 @@
         <v>633</v>
       </c>
       <c r="I29" s="30" t="s">
-        <v>3361</v>
+        <v>3359</v>
       </c>
       <c r="J29" s="30" t="s">
-        <v>3386</v>
+        <v>3384</v>
       </c>
       <c r="M29" s="30" t="s">
         <v>634</v>
@@ -31995,7 +31989,7 @@
         <v>635</v>
       </c>
       <c r="AN29" s="30" t="s">
-        <v>3331</v>
+        <v>3329</v>
       </c>
       <c r="AR29" s="30" t="s">
         <v>636</v>
@@ -32004,7 +31998,7 @@
         <v>2689</v>
       </c>
       <c r="CH29" s="30" t="s">
-        <v>3329</v>
+        <v>3327</v>
       </c>
       <c r="DG29" s="30" t="s">
         <v>1032</v>
@@ -32027,10 +32021,10 @@
         <v>640</v>
       </c>
       <c r="I30" s="30" t="s">
-        <v>3362</v>
+        <v>3360</v>
       </c>
       <c r="J30" s="30" t="s">
-        <v>3387</v>
+        <v>3385</v>
       </c>
       <c r="M30" s="30" t="s">
         <v>641</v>
@@ -39976,9 +39970,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
-      <selection activeCell="D16" pane="topRight" sqref="D16"/>
+      <selection activeCell="B3" pane="topRight" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -40012,7 +40006,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>3306</v>
+        <v>3304</v>
       </c>
     </row>
     <row customFormat="1" r="3" s="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -40020,7 +40014,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>3429</v>
+        <v>3424</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>2577</v>
@@ -40093,7 +40087,7 @@
     </row>
     <row customFormat="1" r="8" s="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="60" t="s">
-        <v>3258</v>
+        <v>3256</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>3192</v>
@@ -40124,7 +40118,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>3406</v>
+        <v>3403</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>90</v>
@@ -40242,10 +40236,10 @@
     </row>
     <row customFormat="1" r="18" s="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="60" t="s">
-        <v>3259</v>
+        <v>3257</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>3422</v>
+        <v>3417</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>2554</v>
@@ -40261,7 +40255,7 @@
         <v>51</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>3407</v>
+        <v>3404</v>
       </c>
       <c r="F20" s="19" t="s">
         <v>2555</v>
@@ -40272,7 +40266,7 @@
         <v>53</v>
       </c>
       <c r="B21" s="86" t="s">
-        <v>3408</v>
+        <v>3405</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>2556</v>
@@ -40380,7 +40374,7 @@
         <v>74</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>3409</v>
+        <v>3406</v>
       </c>
       <c r="F28" s="19" t="s">
         <v>2557</v>
@@ -40391,7 +40385,7 @@
         <v>76</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>3295</v>
+        <v>3293</v>
       </c>
       <c r="F29" s="2" t="s">
         <v>78</v>
@@ -40402,7 +40396,7 @@
         <v>82</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>3295</v>
+        <v>3293</v>
       </c>
       <c r="F30" s="2" t="s">
         <v>78</v>
@@ -40413,7 +40407,7 @@
         <v>107</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>3296</v>
+        <v>3294</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>85</v>
@@ -40424,7 +40418,7 @@
         <v>88</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>3298</v>
+        <v>3296</v>
       </c>
       <c r="F32" s="19" t="s">
         <v>215</v>
@@ -40435,7 +40429,7 @@
         <v>86</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>3297</v>
+        <v>3295</v>
       </c>
       <c r="F33" s="19" t="s">
         <v>215</v>
@@ -40446,7 +40440,7 @@
         <v>89</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>3299</v>
+        <v>3297</v>
       </c>
       <c r="F34" s="19" t="s">
         <v>2562</v>
@@ -40672,7 +40666,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
-      <selection activeCell="D2" pane="topRight" sqref="D2"/>
+      <selection activeCell="B2" pane="topRight" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -41079,7 +41073,7 @@
         <v>16</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>3404</v>
+        <v>3402</v>
       </c>
       <c r="C6" s="51" t="s">
         <v>3229</v>
@@ -41114,7 +41108,7 @@
     </row>
     <row customFormat="1" r="7" s="50" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A7" s="64" t="s">
-        <v>3258</v>
+        <v>3256</v>
       </c>
       <c r="B7" s="52"/>
       <c r="C7" s="52" t="s">
@@ -41173,13 +41167,13 @@
         <v>31</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>3423</v>
+        <v>3418</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>3311</v>
+        <v>3309</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>3312</v>
+        <v>3310</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>32</v>
@@ -41193,7 +41187,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>3397</v>
+        <v>3395</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>34</v>
@@ -41332,7 +41326,7 @@
       </c>
       <c r="C12" s="72"/>
       <c r="D12" s="73" t="s">
-        <v>3313</v>
+        <v>3311</v>
       </c>
       <c r="E12" s="72"/>
       <c r="F12" s="72"/>
@@ -41382,13 +41376,13 @@
         <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>3424</v>
+        <v>3419</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>3314</v>
+        <v>3312</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>3315</v>
+        <v>3313</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>41</v>
@@ -41721,19 +41715,19 @@
     </row>
     <row customFormat="1" r="21" s="19" spans="1:101" x14ac:dyDescent="0.25">
       <c r="A21" s="60" t="s">
-        <v>3259</v>
+        <v>3257</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>3425</v>
+        <v>3420</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>3336</v>
+        <v>3334</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>3317</v>
+        <v>3315</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>3316</v>
+        <v>3314</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>49</v>
@@ -41848,13 +41842,13 @@
         <v>51</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>3389</v>
+        <v>3387</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>3318</v>
+        <v>3316</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>3319</v>
+        <v>3317</v>
       </c>
       <c r="E23" s="19" t="s">
         <v>52</v>
@@ -41868,13 +41862,13 @@
         <v>53</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>3390</v>
+        <v>3388</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>3320</v>
+        <v>3318</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>3321</v>
+        <v>3319</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>54</v>
@@ -42070,7 +42064,7 @@
         <v>65</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>3339</v>
+        <v>3337</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>66</v>
@@ -43091,7 +43085,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
-      <selection activeCell="D2" pane="topRight" sqref="D2"/>
+      <selection activeCell="B13" pane="topRight" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43201,7 +43195,7 @@
     </row>
     <row customFormat="1" r="7" s="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="60" t="s">
-        <v>3258</v>
+        <v>3256</v>
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="2" t="s">
@@ -43238,13 +43232,13 @@
         <v>98</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>3391</v>
+        <v>3389</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>99</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>3322</v>
+        <v>3320</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>100</v>
@@ -43297,7 +43291,9 @@
       <c r="A12" s="19" t="s">
         <v>2624</v>
       </c>
-      <c r="B12" s="72"/>
+      <c r="B12" s="72">
+        <v>45906</v>
+      </c>
       <c r="D12" s="2" t="s">
         <v>2625</v>
       </c>
@@ -43333,7 +43329,7 @@
         <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>3293</v>
+        <v>3291</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>101</v>
@@ -43410,10 +43406,10 @@
     </row>
     <row customFormat="1" r="18" s="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="60" t="s">
-        <v>3259</v>
+        <v>3257</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>3392</v>
+        <v>3390</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>102</v>
@@ -43439,7 +43435,7 @@
         <v>51</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>3393</v>
+        <v>3391</v>
       </c>
       <c r="C20" s="19" t="s">
         <v>103</v>
@@ -43459,7 +43455,7 @@
         <v>53</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>3394</v>
+        <v>3392</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>54</v>
@@ -43590,7 +43586,7 @@
         <v>74</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>3282</v>
+        <v>3280</v>
       </c>
     </row>
     <row customFormat="1" r="30" s="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -43598,7 +43594,7 @@
         <v>76</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>3281</v>
+        <v>3279</v>
       </c>
     </row>
     <row customFormat="1" r="31" s="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -43855,7 +43851,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
-      <selection activeCell="D2" pane="topRight" sqref="D2"/>
+      <selection activeCell="D5" pane="topRight" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43916,7 +43912,7 @@
         <v>2559</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>2560</v>
+        <v>2561</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>2561</v>
@@ -43942,28 +43938,22 @@
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
-      <c r="D5" s="19" t="s">
-        <v>3237</v>
-      </c>
+      <c r="D5" s="19"/>
       <c r="E5" s="19"/>
       <c r="F5" s="19" t="s">
-        <v>3238</v>
+        <v>3237</v>
       </c>
     </row>
     <row customFormat="1" r="6" s="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="83" t="s">
-        <v>3405</v>
-      </c>
+      <c r="B6" s="19"/>
       <c r="C6" s="19"/>
-      <c r="D6" s="19" t="s">
-        <v>3239</v>
-      </c>
+      <c r="D6" s="19"/>
       <c r="E6" s="19"/>
       <c r="F6" s="19" t="s">
-        <v>3240</v>
+        <v>3238</v>
       </c>
     </row>
     <row customFormat="1" r="7" s="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -43991,13 +43981,13 @@
         <v>98</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>3395</v>
+        <v>3393</v>
       </c>
       <c r="C8" s="19" t="s">
+        <v>3321</v>
+      </c>
+      <c r="D8" s="19" t="s">
         <v>3323</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>3325</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>2564</v>
@@ -44011,16 +44001,16 @@
         <v>50</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>3396</v>
+        <v>3394</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>3322</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>3324</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>3326</v>
-      </c>
       <c r="E9" s="2" t="s">
-        <v>3292</v>
+        <v>3290</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>112</v>
@@ -44096,7 +44086,7 @@
         <v>74</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>3283</v>
+        <v>3281</v>
       </c>
     </row>
     <row customFormat="1" r="15" s="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -44172,7 +44162,7 @@
     <mergeCell ref="A4:XFD4"/>
     <mergeCell ref="A12:XFD12"/>
   </mergeCells>
-  <conditionalFormatting sqref="A5:XFD5 A6 C6:XFD6">
+  <conditionalFormatting sqref="B6:XFD6 A5:XFD5">
     <cfRule dxfId="110" priority="3" type="expression">
       <formula>A$3="Input Data"</formula>
     </cfRule>
@@ -44239,7 +44229,7 @@
     <dataValidation showErrorMessage="1" showInputMessage="1" sqref="C21" type="list">
       <formula1>ListOwnership</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="C5:C6" type="custom">
+    <dataValidation allowBlank="1" showErrorMessage="1" showInputMessage="1" sqref="B6:D6 C5:D5" type="custom">
       <formula1>B$3="LookUp"</formula1>
     </dataValidation>
   </dataValidations>
@@ -44290,9 +44280,9 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
-      <selection activeCell="B7" pane="topRight" sqref="B7"/>
+      <selection activeCell="B8" pane="topRight" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44323,9 +44313,9 @@
       <c r="A2" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="19" t="str">
+      <c r="B2" s="53" t="str">
         <f>'1.TabCustomerMainData'!$B$3</f>
-        <v>0002APP20211202563</v>
+        <v>0002APP20211202680</v>
       </c>
     </row>
     <row customFormat="1" r="3" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -44333,7 +44323,7 @@
         <v>16</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>3421</v>
+        <v>3229</v>
       </c>
     </row>
     <row customFormat="1" r="4" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -44341,7 +44331,7 @@
         <v>2572</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>3388</v>
+        <v>3386</v>
       </c>
     </row>
     <row customFormat="1" r="5" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -44349,7 +44339,7 @@
         <v>2573</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>3419</v>
+        <v>3416</v>
       </c>
     </row>
     <row customFormat="1" r="6" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -44357,7 +44347,7 @@
         <v>2574</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>3426</v>
+        <v>3421</v>
       </c>
     </row>
     <row customFormat="1" r="7" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -44365,7 +44355,7 @@
         <v>2575</v>
       </c>
       <c r="B7" s="83" t="s">
-        <v>3427</v>
+        <v>3426</v>
       </c>
     </row>
     <row customFormat="1" r="8" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -44373,7 +44363,7 @@
         <v>2576</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>3420</v>
+        <v>3423</v>
       </c>
     </row>
     <row ht="49.5" r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -44381,7 +44371,7 @@
         <v>190</v>
       </c>
       <c r="B10" s="71" t="s">
-        <v>3260</v>
+        <v>3258</v>
       </c>
     </row>
   </sheetData>
@@ -44428,22 +44418,22 @@
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>3275</v>
+        <v>3273</v>
       </c>
       <c r="E1" t="s">
-        <v>3275</v>
+        <v>3273</v>
       </c>
       <c r="F1" t="s">
-        <v>3275</v>
+        <v>3273</v>
       </c>
       <c r="G1" t="s">
-        <v>3275</v>
+        <v>3273</v>
       </c>
       <c r="H1" t="s">
-        <v>3275</v>
+        <v>3273</v>
       </c>
       <c r="I1" t="s">
-        <v>3275</v>
+        <v>3273</v>
       </c>
       <c r="J1" t="s">
         <v>10</v>
@@ -44495,25 +44485,25 @@
         <v>17</v>
       </c>
       <c r="D4" s="19" t="s">
+        <v>3268</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>3267</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>3271</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>3272</v>
+      </c>
+      <c r="H4" s="19" t="s">
+        <v>3269</v>
+      </c>
+      <c r="I4" s="19" t="s">
         <v>3270</v>
       </c>
-      <c r="E4" s="19" t="s">
-        <v>3269</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>3273</v>
-      </c>
-      <c r="G4" s="19" t="s">
-        <v>3274</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>3271</v>
-      </c>
-      <c r="I4" s="19" t="s">
-        <v>3272</v>
-      </c>
       <c r="J4" s="19" t="s">
-        <v>3272</v>
+        <v>3270</v>
       </c>
     </row>
     <row customFormat="1" r="5" s="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -44611,7 +44601,7 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>3275</v>
+        <v>3273</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>24</v>
@@ -44646,7 +44636,7 @@
         <v>127</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>3300</v>
+        <v>3298</v>
       </c>
     </row>
     <row customFormat="1" r="6" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -44767,7 +44757,7 @@
         <v>74</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>3403</v>
+        <v>3401</v>
       </c>
     </row>
     <row customFormat="1" r="23" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -44799,7 +44789,7 @@
         <v>88</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>3298</v>
+        <v>3296</v>
       </c>
     </row>
     <row customFormat="1" r="27" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -44807,7 +44797,7 @@
         <v>86</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>3297</v>
+        <v>3295</v>
       </c>
     </row>
     <row customFormat="1" r="28" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -44815,7 +44805,7 @@
         <v>152</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>3399</v>
+        <v>3397</v>
       </c>
     </row>
     <row customFormat="1" r="29" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -45122,7 +45112,7 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>3275</v>
+        <v>3273</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>24</v>
@@ -45154,7 +45144,7 @@
         <v>180</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>3301</v>
+        <v>3299</v>
       </c>
     </row>
     <row customFormat="1" r="5" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -45162,7 +45152,7 @@
         <v>182</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>3302</v>
+        <v>3300</v>
       </c>
     </row>
     <row customFormat="1" r="6" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -45170,7 +45160,7 @@
         <v>183</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>3303</v>
+        <v>3301</v>
       </c>
     </row>
     <row customFormat="1" r="7" s="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -45184,10 +45174,10 @@
     </row>
     <row customFormat="1" r="8" s="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="59" t="s">
-        <v>3307</v>
+        <v>3305</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>3308</v>
+        <v>3306</v>
       </c>
     </row>
     <row customFormat="1" r="9" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -45195,7 +45185,7 @@
         <v>184</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>3417</v>
+        <v>3414</v>
       </c>
     </row>
     <row customFormat="1" r="10" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -45211,7 +45201,7 @@
         <v>186</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>3410</v>
+        <v>3407</v>
       </c>
     </row>
     <row customFormat="1" r="12" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -45219,7 +45209,7 @@
         <v>187</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>3411</v>
+        <v>3408</v>
       </c>
     </row>
     <row customFormat="1" r="13" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -45227,7 +45217,7 @@
         <v>188</v>
       </c>
       <c r="B13" s="87" t="s">
-        <v>3412</v>
+        <v>3409</v>
       </c>
     </row>
     <row customFormat="1" r="14" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -45297,12 +45287,12 @@
         <v>198</v>
       </c>
       <c r="B22" s="84" t="s">
-        <v>3418</v>
+        <v>3415</v>
       </c>
     </row>
     <row customFormat="1" r="23" s="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="59" t="s">
-        <v>3279</v>
+        <v>3277</v>
       </c>
       <c r="B23" s="84">
         <v>527245</v>
@@ -45310,7 +45300,7 @@
     </row>
     <row customFormat="1" r="24" s="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="59" t="s">
-        <v>3280</v>
+        <v>3278</v>
       </c>
       <c r="B24" s="7"/>
     </row>
@@ -45325,7 +45315,7 @@
         <v>199</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>3304</v>
+        <v>3302</v>
       </c>
     </row>
     <row customFormat="1" r="27" s="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -45347,7 +45337,7 @@
         <v>201</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>3294</v>
+        <v>3292</v>
       </c>
     </row>
     <row customFormat="1" r="30" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -45385,7 +45375,7 @@
         <v>205</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>3400</v>
+        <v>3398</v>
       </c>
     </row>
     <row customFormat="1" r="35" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -45431,7 +45421,7 @@
         <v>211</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>3398</v>
+        <v>3396</v>
       </c>
     </row>
     <row customFormat="1" r="41" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -45463,7 +45453,7 @@
         <v>74</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>3401</v>
+        <v>3399</v>
       </c>
     </row>
     <row customFormat="1" r="45" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -45495,7 +45485,7 @@
         <v>88</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>3298</v>
+        <v>3296</v>
       </c>
     </row>
     <row customFormat="1" r="49" s="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -45503,7 +45493,7 @@
         <v>86</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>3297</v>
+        <v>3295</v>
       </c>
     </row>
     <row customFormat="1" r="50" s="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -45511,7 +45501,7 @@
         <v>89</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>3399</v>
+        <v>3397</v>
       </c>
     </row>
     <row customFormat="1" r="51" s="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -45541,7 +45531,7 @@
         <v>74</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>3401</v>
+        <v>3399</v>
       </c>
     </row>
     <row customFormat="1" r="55" s="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -45573,7 +45563,7 @@
         <v>86</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>3298</v>
+        <v>3296</v>
       </c>
     </row>
     <row customFormat="1" r="59" s="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -45581,7 +45571,7 @@
         <v>88</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>3297</v>
+        <v>3295</v>
       </c>
     </row>
     <row customFormat="1" r="60" s="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -45589,18 +45579,18 @@
         <v>89</v>
       </c>
       <c r="B60" s="19" t="s">
-        <v>3399</v>
+        <v>3397</v>
       </c>
     </row>
     <row customFormat="1" r="61" s="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="93" t="s">
-        <v>3327</v>
+        <v>3325</v>
       </c>
       <c r="B61" s="94"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="82" t="s">
-        <v>3328</v>
+        <v>3326</v>
       </c>
       <c r="B62" s="39" t="s">
         <v>73</v>

</xml_diff>

<commit_message>
AITATR3-39 NAP 2 - Tab Financial Data - Verify Calculation
</commit_message>
<xml_diff>
--- a/Excel/2. DataFile_NAP_CF4W.xlsx
+++ b/Excel/2. DataFile_NAP_CF4W.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="17" firstSheet="14" tabRatio="769" windowHeight="7650" windowWidth="20490" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="12" firstSheet="7" tabRatio="769" windowHeight="7650" windowWidth="20490" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="0.Setting" r:id="rId1" sheetId="5"/>
@@ -14444,7 +14444,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4277" uniqueCount="3436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4223" uniqueCount="3427">
   <si>
     <t>Count</t>
   </si>
@@ -24692,12 +24692,6 @@
     <t>1000;1000;1000;1000;1000;1000</t>
   </si>
   <si>
-    <t>Used</t>
-  </si>
-  <si>
-    <t>KB1010RFO</t>
-  </si>
-  <si>
     <t>FT DAVID;Ft janu;ft HANDY</t>
   </si>
   <si>
@@ -24725,40 +24719,19 @@
     <t>New;Select Similardata;Select ApplicationInProccess</t>
   </si>
   <si>
-    <t>0002APP20211202752</t>
-  </si>
-  <si>
     <t>New;Select Similardata;Select ApplicationInProccess;select Similardata;Select ApplicationInProccess;Select ApplicationInProccess</t>
   </si>
   <si>
     <t>FT RICKY</t>
   </si>
   <si>
-    <t>FT JOY;FT SANI;DOGE MOTHER;FT BOD;FT EMP</t>
-  </si>
-  <si>
-    <t>0002APP20211202759</t>
-  </si>
-  <si>
-    <t>0002APP20211202764</t>
-  </si>
-  <si>
-    <t>null;FT JOY;FT JOY;FT ANDRI;FT ANDRI;null;FT BOD;FT BOD;FT EMP;FT EMP</t>
-  </si>
-  <si>
-    <t>0002APP20211202765</t>
-  </si>
-  <si>
-    <t>null;FT JOY;DOGE BOTHER;null;FT BOD;FT EMP</t>
-  </si>
-  <si>
-    <t>0002APP20211202770</t>
-  </si>
-  <si>
     <t>FT JOY;FT SANI;DOGE BOTHER;FT BOD;FT EMP</t>
   </si>
   <si>
     <t>0002APP20211202771</t>
+  </si>
+  <si>
+    <t>New</t>
   </si>
 </sst>
 </file>
@@ -28314,8 +28287,8 @@
   <sheetPr codeName="Sheet20"/>
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28546,7 +28519,7 @@
         <v>292</v>
       </c>
       <c r="B29" s="19">
-        <v>26.6</v>
+        <v>8.6999999999999993</v>
       </c>
     </row>
     <row customFormat="1" r="30" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -28833,7 +28806,7 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>3273</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>24</v>
@@ -29546,7 +29519,7 @@
   <sheetPr codeName="Sheet18"/>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
       <selection activeCell="A7" pane="topRight" sqref="A7"/>
     </sheetView>
@@ -29589,7 +29562,7 @@
         <v>119</v>
       </c>
       <c r="B3" t="s">
-        <v>3426</v>
+        <v>3423</v>
       </c>
     </row>
     <row customFormat="1" r="4" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -29605,7 +29578,7 @@
         <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>3420</v>
+        <v>3418</v>
       </c>
     </row>
     <row customFormat="1" r="6" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -29621,7 +29594,7 @@
         <v>2581</v>
       </c>
       <c r="B7" t="s">
-        <v>3434</v>
+        <v>3424</v>
       </c>
     </row>
     <row customFormat="1" r="8" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -40052,7 +40025,7 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>3435</v>
+        <v>3425</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>2577</v>
@@ -40277,7 +40250,7 @@
         <v>3257</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>3416</v>
+        <v>3414</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>2554</v>
@@ -41205,7 +41178,7 @@
         <v>31</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>3417</v>
+        <v>3415</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>3309</v>
@@ -41414,7 +41387,7 @@
         <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>3418</v>
+        <v>3416</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>3312</v>
@@ -41756,7 +41729,7 @@
         <v>3257</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>3419</v>
+        <v>3417</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>3334</v>
@@ -44369,7 +44342,7 @@
         <v>2572</v>
       </c>
       <c r="B4" s="88" t="s">
-        <v>3422</v>
+        <v>3420</v>
       </c>
     </row>
     <row customFormat="1" r="5" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -44377,7 +44350,7 @@
         <v>2573</v>
       </c>
       <c r="B5" s="88" t="s">
-        <v>3415</v>
+        <v>3413</v>
       </c>
     </row>
     <row customFormat="1" ht="30" r="6" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -44385,7 +44358,7 @@
         <v>2574</v>
       </c>
       <c r="B6" s="88" t="s">
-        <v>3423</v>
+        <v>3421</v>
       </c>
     </row>
     <row customFormat="1" ht="28.5" r="7" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -44393,7 +44366,7 @@
         <v>2575</v>
       </c>
       <c r="B7" s="89" t="s">
-        <v>3421</v>
+        <v>3419</v>
       </c>
     </row>
     <row customFormat="1" ht="75" r="8" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -44401,7 +44374,7 @@
         <v>2576</v>
       </c>
       <c r="B8" s="88" t="s">
-        <v>3425</v>
+        <v>3422</v>
       </c>
     </row>
     <row ht="49.5" r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -44620,10 +44593,10 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
       <selection activeCell="A34" sqref="A34"/>
-      <selection activeCell="B51" pane="topRight" sqref="B51"/>
+      <selection activeCell="B16" pane="topRight" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44639,7 +44612,7 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>3273</v>
+        <v>10</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>24</v>
@@ -44753,7 +44726,7 @@
         <v>144</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>332</v>
+        <v>358</v>
       </c>
     </row>
     <row customFormat="1" r="17" s="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -45135,7 +45108,7 @@
     <sheetView topLeftCell="A7" workbookViewId="0">
       <pane activePane="topRight" state="frozen" topLeftCell="B1" xSplit="1"/>
       <selection activeCell="A43" sqref="A43"/>
-      <selection activeCell="B14" pane="topRight" sqref="B14"/>
+      <selection activeCell="B9" pane="topRight" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45150,7 +45123,7 @@
         <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>3273</v>
+        <v>10</v>
       </c>
       <c r="C1" s="19" t="s">
         <v>24</v>
@@ -45223,7 +45196,7 @@
         <v>184</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>3413</v>
+        <v>3426</v>
       </c>
     </row>
     <row customFormat="1" r="10" s="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -45308,33 +45281,25 @@
       <c r="A20" s="59" t="s">
         <v>196</v>
       </c>
-      <c r="B20" s="83">
-        <v>75346</v>
-      </c>
+      <c r="B20" s="83"/>
     </row>
     <row customFormat="1" r="21" s="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="59" t="s">
         <v>197</v>
       </c>
-      <c r="B21" s="83">
-        <v>82364</v>
-      </c>
+      <c r="B21" s="83"/>
     </row>
     <row customFormat="1" r="22" s="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="59" t="s">
         <v>198</v>
       </c>
-      <c r="B22" s="83" t="s">
-        <v>3414</v>
-      </c>
+      <c r="B22" s="83"/>
     </row>
     <row customFormat="1" r="23" s="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="59" t="s">
         <v>3277</v>
       </c>
-      <c r="B23" s="83">
-        <v>527245</v>
-      </c>
+      <c r="B23" s="83"/>
     </row>
     <row customFormat="1" r="24" s="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="59" t="s">

</xml_diff>

<commit_message>
Penamabahan isjoinincome cdc personal tabfinancial
</commit_message>
<xml_diff>
--- a/Excel/2. DataFile_NAP_CF4W.xlsx
+++ b/Excel/2. DataFile_NAP_CF4W.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="15705" windowHeight="5820" tabRatio="769" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15705" windowHeight="5820" tabRatio="769" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="0.Setting" sheetId="5" r:id="rId1"/>
@@ -14445,7 +14445,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4226" uniqueCount="3435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4231" uniqueCount="3435">
   <si>
     <t>Count</t>
   </si>
@@ -41444,9 +41444,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:CW51"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C47" sqref="C47"/>
+      <selection pane="topRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43874,10 +43874,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43886,21 +43886,132 @@
     <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="90" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="19" t="str">
-        <f>'1.TabCustomerMainData'!$B$3</f>
+        <f>'1.TabCustomerMainData'!B$3</f>
         <v>0002APP20211202964</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="19" t="str">
+        <f>'1.TabCustomerMainData'!C$3</f>
+        <v>0002APP20211201264</v>
+      </c>
+      <c r="D2" s="19" t="str">
+        <f>'1.TabCustomerMainData'!D$3</f>
+        <v>0002APP20211201270</v>
+      </c>
+      <c r="E2" s="19" t="str">
+        <f>'1.TabCustomerMainData'!E$3</f>
+        <v>0002APP20211201271</v>
+      </c>
+      <c r="F2" s="19" t="str">
+        <f>'1.TabCustomerMainData'!F$3</f>
+        <v>0002APP20211201272</v>
+      </c>
+      <c r="G2" s="19">
+        <f>'1.TabCustomerMainData'!G$3</f>
+        <v>0</v>
+      </c>
+      <c r="H2" s="19">
+        <f>'1.TabCustomerMainData'!H$3</f>
+        <v>0</v>
+      </c>
+      <c r="I2" s="19">
+        <f>'1.TabCustomerMainData'!I$3</f>
+        <v>0</v>
+      </c>
+      <c r="J2" s="19">
+        <f>'1.TabCustomerMainData'!J$3</f>
+        <v>0</v>
+      </c>
+      <c r="K2" s="19">
+        <f>'1.TabCustomerMainData'!K$3</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="19">
+        <f>'1.TabCustomerMainData'!L$3</f>
+        <v>0</v>
+      </c>
+      <c r="M2" s="19">
+        <f>'1.TabCustomerMainData'!M$3</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="19">
+        <f>'1.TabCustomerMainData'!N$3</f>
+        <v>0</v>
+      </c>
+      <c r="O2" s="19">
+        <f>'1.TabCustomerMainData'!O$3</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="19">
+        <f>'1.TabCustomerMainData'!P$3</f>
+        <v>0</v>
+      </c>
+      <c r="Q2" s="19">
+        <f>'1.TabCustomerMainData'!Q$3</f>
+        <v>0</v>
+      </c>
+      <c r="R2" s="19">
+        <f>'1.TabCustomerMainData'!R$3</f>
+        <v>0</v>
+      </c>
+      <c r="S2" s="19">
+        <f>'1.TabCustomerMainData'!S$3</f>
+        <v>0</v>
+      </c>
+      <c r="T2" s="19">
+        <f>'1.TabCustomerMainData'!T$3</f>
+        <v>0</v>
+      </c>
+      <c r="U2" s="19">
+        <f>'1.TabCustomerMainData'!U$3</f>
+        <v>0</v>
+      </c>
+      <c r="V2" s="19">
+        <f>'1.TabCustomerMainData'!V$3</f>
+        <v>0</v>
+      </c>
+      <c r="W2" s="19">
+        <f>'1.TabCustomerMainData'!W$3</f>
+        <v>0</v>
+      </c>
+      <c r="X2" s="19">
+        <f>'1.TabCustomerMainData'!X$3</f>
+        <v>0</v>
+      </c>
+      <c r="Y2" s="19">
+        <f>'1.TabCustomerMainData'!Y$3</f>
+        <v>0</v>
+      </c>
+      <c r="Z2" s="19">
+        <f>'1.TabCustomerMainData'!Z$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>190</v>
       </c>

</xml_diff>

<commit_message>
Penambahan cell reason failed & objective
</commit_message>
<xml_diff>
--- a/Excel/2. DataFile_NAP_CF4W.xlsx
+++ b/Excel/2. DataFile_NAP_CF4W.xlsx
@@ -14973,7 +14973,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4307" uniqueCount="3495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4341" uniqueCount="3497">
   <si>
     <t>Count</t>
   </si>
@@ -25465,6 +25465,12 @@
   </si>
   <si>
     <t>TONI;CV SEJAHTERA</t>
+  </si>
+  <si>
+    <t>Reason Failed</t>
+  </si>
+  <si>
+    <t>Objective</t>
   </si>
 </sst>
 </file>
@@ -26137,6 +26143,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -26161,6 +26168,7 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -26215,8 +26223,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -28262,7 +28268,7 @@
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A43" sqref="A43"/>
-      <selection pane="topRight" sqref="A1:XFD10"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28289,8 +28295,16 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>3496</v>
+      </c>
+    </row>
     <row r="4" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -28298,14 +28312,14 @@
     <row r="8" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" s="148" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="118" t="s">
+    <row r="11" spans="1:5" s="121" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="119" t="s">
         <v>3201</v>
       </c>
-      <c r="B11" s="119"/>
-      <c r="C11" s="119"/>
-      <c r="D11" s="119"/>
-      <c r="E11" s="119"/>
+      <c r="B11" s="120"/>
+      <c r="C11" s="120"/>
+      <c r="D11" s="120"/>
+      <c r="E11" s="120"/>
     </row>
     <row r="12" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="59" t="s">
@@ -28337,14 +28351,14 @@
         <v>3283</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="118" t="s">
+    <row r="16" spans="1:5" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="119" t="s">
         <v>3202</v>
       </c>
-      <c r="B16" s="119"/>
-      <c r="C16" s="119"/>
-      <c r="D16" s="119"/>
-      <c r="E16" s="119"/>
+      <c r="B16" s="120"/>
+      <c r="C16" s="120"/>
+      <c r="D16" s="120"/>
+      <c r="E16" s="120"/>
     </row>
     <row r="17" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="59" t="s">
@@ -28470,11 +28484,11 @@
       </c>
       <c r="B33" s="7"/>
     </row>
-    <row r="34" spans="1:2" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="118" t="s">
+    <row r="34" spans="1:2" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="119" t="s">
         <v>3203</v>
       </c>
-      <c r="B34" s="119"/>
+      <c r="B34" s="120"/>
     </row>
     <row r="35" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="59" t="s">
@@ -28484,11 +28498,11 @@
         <v>3284</v>
       </c>
     </row>
-    <row r="36" spans="1:2" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="118" t="s">
+    <row r="36" spans="1:2" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="119" t="s">
         <v>3204</v>
       </c>
-      <c r="B36" s="119"/>
+      <c r="B36" s="120"/>
     </row>
     <row r="37" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
@@ -28514,11 +28528,11 @@
         <v>415</v>
       </c>
     </row>
-    <row r="40" spans="1:2" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="118" t="s">
+    <row r="40" spans="1:2" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="119" t="s">
         <v>3205</v>
       </c>
-      <c r="B40" s="119"/>
+      <c r="B40" s="120"/>
     </row>
     <row r="41" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
@@ -28670,11 +28684,11 @@
         <v>3368</v>
       </c>
     </row>
-    <row r="60" spans="1:2" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="118" t="s">
+    <row r="60" spans="1:2" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="119" t="s">
         <v>3206</v>
       </c>
-      <c r="B60" s="119"/>
+      <c r="B60" s="120"/>
     </row>
     <row r="61" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="58" t="s">
@@ -28748,11 +28762,11 @@
         <v>3368</v>
       </c>
     </row>
-    <row r="70" spans="1:8" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="118" t="s">
+    <row r="70" spans="1:8" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="119" t="s">
         <v>3305</v>
       </c>
-      <c r="B70" s="119"/>
+      <c r="B70" s="120"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="82" t="s">
@@ -28977,7 +28991,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:XFD10"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29015,8 +29029,16 @@
         <v>3268</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>3496</v>
+      </c>
+    </row>
     <row r="4" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -29237,7 +29259,7 @@
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A10" sqref="A10"/>
-      <selection pane="topRight" sqref="A1:XFD10"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29265,8 +29287,16 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>3496</v>
+      </c>
+    </row>
     <row r="4" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -29274,14 +29304,14 @@
     <row r="8" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="127" t="s">
+    <row r="11" spans="1:5" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="129" t="s">
         <v>3207</v>
       </c>
-      <c r="B11" s="128"/>
-      <c r="C11" s="128"/>
-      <c r="D11" s="128"/>
-      <c r="E11" s="129"/>
+      <c r="B11" s="130"/>
+      <c r="C11" s="130"/>
+      <c r="D11" s="130"/>
+      <c r="E11" s="131"/>
     </row>
     <row r="12" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="59" t="s">
@@ -29291,14 +29321,14 @@
         <v>219</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="133" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="130" t="s">
+    <row r="13" spans="1:5" s="135" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="132" t="s">
         <v>118</v>
       </c>
-      <c r="B13" s="131"/>
-      <c r="C13" s="131"/>
-      <c r="D13" s="131"/>
-      <c r="E13" s="132"/>
+      <c r="B13" s="133"/>
+      <c r="C13" s="133"/>
+      <c r="D13" s="133"/>
+      <c r="E13" s="134"/>
     </row>
     <row r="14" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="60" t="s">
@@ -29347,14 +29377,14 @@
         <v>226</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="133" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="130" t="s">
+    <row r="21" spans="1:5" s="135" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="132" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="131"/>
-      <c r="C21" s="131"/>
-      <c r="D21" s="131"/>
-      <c r="E21" s="132"/>
+      <c r="B21" s="133"/>
+      <c r="C21" s="133"/>
+      <c r="D21" s="133"/>
+      <c r="E21" s="134"/>
     </row>
     <row r="22" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="60" t="s">
@@ -29409,14 +29439,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:5" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="127" t="s">
+    <row r="29" spans="1:5" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="129" t="s">
         <v>3208</v>
       </c>
-      <c r="B29" s="128"/>
-      <c r="C29" s="128"/>
-      <c r="D29" s="128"/>
-      <c r="E29" s="129"/>
+      <c r="B29" s="130"/>
+      <c r="C29" s="130"/>
+      <c r="D29" s="130"/>
+      <c r="E29" s="131"/>
     </row>
     <row r="30" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="65" t="s">
@@ -29442,14 +29472,14 @@
         <v>800000</v>
       </c>
     </row>
-    <row r="33" spans="1:5" s="137" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="134" t="s">
+    <row r="33" spans="1:5" s="139" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="136" t="s">
         <v>3209</v>
       </c>
-      <c r="B33" s="135"/>
-      <c r="C33" s="135"/>
-      <c r="D33" s="135"/>
-      <c r="E33" s="136"/>
+      <c r="B33" s="137"/>
+      <c r="C33" s="137"/>
+      <c r="D33" s="137"/>
+      <c r="E33" s="138"/>
     </row>
     <row r="34" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="60" t="s">
@@ -29459,14 +29489,14 @@
         <v>239</v>
       </c>
     </row>
-    <row r="35" spans="1:5" s="130" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="130" t="s">
+    <row r="35" spans="1:5" s="132" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="132" t="s">
         <v>240</v>
       </c>
-      <c r="B35" s="131"/>
-      <c r="C35" s="131"/>
-      <c r="D35" s="131"/>
-      <c r="E35" s="131"/>
+      <c r="B35" s="133"/>
+      <c r="C35" s="133"/>
+      <c r="D35" s="133"/>
+      <c r="E35" s="133"/>
     </row>
     <row r="36" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
@@ -29535,14 +29565,14 @@
       <c r="D43" s="104"/>
       <c r="E43" s="104"/>
     </row>
-    <row r="44" spans="1:5" s="138" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="138" t="s">
+    <row r="44" spans="1:5" s="140" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="140" t="s">
         <v>3420</v>
       </c>
-      <c r="B44" s="139"/>
-      <c r="C44" s="139"/>
-      <c r="D44" s="139"/>
-      <c r="E44" s="139"/>
+      <c r="B44" s="141"/>
+      <c r="C44" s="141"/>
+      <c r="D44" s="141"/>
+      <c r="E44" s="141"/>
     </row>
     <row r="45" spans="1:5" s="92" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="92" t="s">
@@ -29576,14 +29606,14 @@
         <v>3408</v>
       </c>
     </row>
-    <row r="49" spans="1:5" s="140" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="140" t="s">
+    <row r="49" spans="1:5" s="142" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="142" t="s">
         <v>240</v>
       </c>
-      <c r="B49" s="141"/>
-      <c r="C49" s="141"/>
-      <c r="D49" s="141"/>
-      <c r="E49" s="141"/>
+      <c r="B49" s="143"/>
+      <c r="C49" s="143"/>
+      <c r="D49" s="143"/>
+      <c r="E49" s="143"/>
     </row>
     <row r="50" spans="1:5" s="92" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="92" t="s">
@@ -29649,8 +29679,8 @@
         <v>3411</v>
       </c>
     </row>
-    <row r="58" spans="1:5" s="142" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="142" t="s">
+    <row r="58" spans="1:5" s="144" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="144" t="s">
         <v>3396</v>
       </c>
     </row>
@@ -29812,11 +29842,11 @@
       </c>
       <c r="B79" s="13"/>
     </row>
-    <row r="80" spans="1:2" s="125" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="125" t="s">
+    <row r="80" spans="1:2" s="127" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="127" t="s">
         <v>3210</v>
       </c>
-      <c r="B80" s="126"/>
+      <c r="B80" s="128"/>
     </row>
     <row r="81" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="19" t="s">
@@ -29835,10 +29865,10 @@
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="121" t="s">
+      <c r="A84" s="123" t="s">
         <v>3405</v>
       </c>
-      <c r="B84" s="122"/>
+      <c r="B84" s="124"/>
     </row>
     <row r="85" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A85" s="98" t="s">
@@ -29850,10 +29880,10 @@
       </c>
     </row>
     <row r="86" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="123" t="s">
+      <c r="A86" s="125" t="s">
         <v>3404</v>
       </c>
-      <c r="B86" s="124"/>
+      <c r="B86" s="126"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="91" t="s">
@@ -29865,14 +29895,14 @@
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="120" t="s">
+      <c r="A88" s="122" t="s">
         <v>3424</v>
       </c>
-      <c r="B88" s="120"/>
+      <c r="B88" s="122"/>
     </row>
     <row r="89" spans="1:2" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="120"/>
-      <c r="B89" s="120"/>
+      <c r="A89" s="122"/>
+      <c r="B89" s="122"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -29996,7 +30026,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D8" sqref="D8"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30025,8 +30055,16 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>3496</v>
+      </c>
+    </row>
     <row r="4" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -30034,8 +30072,8 @@
     <row r="8" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="110" t="s">
+    <row r="11" spans="1:5" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="111" t="s">
         <v>3211</v>
       </c>
     </row>
@@ -30091,8 +30129,8 @@
         <v>255</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="110" t="s">
+    <row r="17" spans="1:3" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="111" t="s">
         <v>3212</v>
       </c>
     </row>
@@ -30140,8 +30178,8 @@
         <v>2614</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="110" t="s">
+    <row r="22" spans="1:3" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="111" t="s">
         <v>3213</v>
       </c>
     </row>
@@ -30249,7 +30287,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD10"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30277,8 +30315,16 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>3496</v>
+      </c>
+    </row>
     <row r="4" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -30286,14 +30332,14 @@
     <row r="8" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="127" t="s">
+    <row r="11" spans="1:5" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="129" t="s">
         <v>3214</v>
       </c>
-      <c r="B11" s="128"/>
-      <c r="C11" s="128"/>
-      <c r="D11" s="128"/>
-      <c r="E11" s="129"/>
+      <c r="B11" s="130"/>
+      <c r="C11" s="130"/>
+      <c r="D11" s="130"/>
+      <c r="E11" s="131"/>
     </row>
     <row r="12" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="66" t="s">
@@ -30333,14 +30379,14 @@
         <v>269</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="127" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="127" t="s">
+    <row r="19" spans="1:5" s="129" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="129" t="s">
         <v>3215</v>
       </c>
-      <c r="B19" s="128"/>
-      <c r="C19" s="128"/>
-      <c r="D19" s="128"/>
-      <c r="E19" s="128"/>
+      <c r="B19" s="130"/>
+      <c r="C19" s="130"/>
+      <c r="D19" s="130"/>
+      <c r="E19" s="130"/>
     </row>
     <row r="20" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="58" t="s">
@@ -30518,14 +30564,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="127" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="127" t="s">
+    <row r="42" spans="1:5" s="129" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="129" t="s">
         <v>3216</v>
       </c>
-      <c r="B42" s="128"/>
-      <c r="C42" s="128"/>
-      <c r="D42" s="128"/>
-      <c r="E42" s="128"/>
+      <c r="B42" s="130"/>
+      <c r="C42" s="130"/>
+      <c r="D42" s="130"/>
+      <c r="E42" s="130"/>
     </row>
     <row r="43" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
@@ -30781,7 +30827,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD10"/>
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30810,11 +30856,15 @@
       </c>
     </row>
     <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
+      <c r="A2" s="19" t="s">
+        <v>3495</v>
+      </c>
       <c r="C2" s="15"/>
     </row>
     <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15"/>
+      <c r="A3" s="19" t="s">
+        <v>3496</v>
+      </c>
       <c r="C3" s="15"/>
     </row>
     <row r="4" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
@@ -30846,9 +30896,9 @@
       <c r="C10" s="15"/>
     </row>
     <row r="11" spans="1:5" s="108" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="149"/>
+      <c r="A11" s="110"/>
       <c r="B11" s="107"/>
-      <c r="C11" s="149"/>
+      <c r="C11" s="110"/>
     </row>
     <row r="12" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
@@ -30905,10 +30955,10 @@
       <c r="C19" s="16"/>
     </row>
     <row r="20" spans="1:3" s="26" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="143" t="s">
+      <c r="A20" s="145" t="s">
         <v>2616</v>
       </c>
-      <c r="B20" s="143"/>
+      <c r="B20" s="145"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -30933,7 +30983,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:XFD9"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -30962,8 +31012,16 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>3496</v>
+      </c>
+    </row>
     <row r="4" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -31051,7 +31109,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:XFD10"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31078,8 +31136,16 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>3496</v>
+      </c>
+    </row>
     <row r="4" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -31098,14 +31164,14 @@
         <v>217</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="125" t="s">
+    <row r="13" spans="1:5" s="147" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="127" t="s">
         <v>2605</v>
       </c>
-      <c r="B13" s="126"/>
-      <c r="C13" s="126"/>
-      <c r="D13" s="126"/>
-      <c r="E13" s="144"/>
+      <c r="B13" s="128"/>
+      <c r="C13" s="128"/>
+      <c r="D13" s="128"/>
+      <c r="E13" s="146"/>
     </row>
     <row r="14" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
@@ -31201,14 +31267,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:5" s="145" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="125" t="s">
+    <row r="26" spans="1:5" s="147" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="127" t="s">
         <v>2609</v>
       </c>
-      <c r="B26" s="126"/>
-      <c r="C26" s="126"/>
-      <c r="D26" s="126"/>
-      <c r="E26" s="144"/>
+      <c r="B26" s="128"/>
+      <c r="C26" s="128"/>
+      <c r="D26" s="128"/>
+      <c r="E26" s="146"/>
     </row>
     <row r="27" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="13" t="s">
@@ -31326,11 +31392,11 @@
         <v>3392</v>
       </c>
     </row>
-    <row r="42" spans="1:2" s="145" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="125" t="s">
+    <row r="42" spans="1:2" s="147" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="127" t="s">
         <v>2593</v>
       </c>
-      <c r="B42" s="126"/>
+      <c r="B42" s="128"/>
     </row>
     <row r="43" spans="1:2" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="19" t="s">
@@ -31411,10 +31477,10 @@
       <c r="B54" s="20"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="146" t="s">
+      <c r="A55" s="148" t="s">
         <v>2597</v>
       </c>
-      <c r="B55" s="147"/>
+      <c r="B55" s="149"/>
     </row>
     <row r="56" spans="1:2" ht="210" x14ac:dyDescent="0.25">
       <c r="A56" s="25" t="s">
@@ -31483,7 +31549,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:XFD10"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31510,8 +31576,16 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>3496</v>
+      </c>
+    </row>
     <row r="4" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -31583,12 +31657,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="L8" sqref="L8"/>
+      <selection pane="topRight" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="5" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
@@ -31610,8 +31684,16 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>3496</v>
+      </c>
+    </row>
     <row r="4" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -31704,7 +31786,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D13" sqref="D13"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31733,8 +31815,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>3495</v>
+      </c>
+    </row>
     <row r="3" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>3496</v>
+      </c>
       <c r="B3"/>
       <c r="M3"/>
     </row>
@@ -31796,8 +31885,8 @@
         <v>2559</v>
       </c>
     </row>
-    <row r="15" spans="1:13" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="110" t="s">
+    <row r="15" spans="1:13" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="111" t="s">
         <v>3190</v>
       </c>
     </row>
@@ -32022,8 +32111,8 @@
         <v>2554</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="110" t="s">
+    <row r="32" spans="1:6" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="111" t="s">
         <v>3191</v>
       </c>
     </row>
@@ -32111,8 +32200,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="110" t="s">
+    <row r="37" spans="1:6" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="111" t="s">
         <v>3192</v>
       </c>
     </row>
@@ -42763,7 +42852,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B12" sqref="B12"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43079,8 +43168,16 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:101" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:101" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:101" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:101" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>3496</v>
+      </c>
+    </row>
     <row r="4" spans="1:101" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:101" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:101" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -44212,110 +44309,110 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:101" s="114" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="111" t="s">
+    <row r="40" spans="1:101" s="115" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="112" t="s">
         <v>3191</v>
       </c>
-      <c r="B40" s="112"/>
-      <c r="C40" s="112"/>
-      <c r="D40" s="112"/>
-      <c r="E40" s="112"/>
-      <c r="F40" s="112"/>
-      <c r="G40" s="112"/>
-      <c r="H40" s="112"/>
-      <c r="I40" s="112"/>
-      <c r="J40" s="112"/>
-      <c r="K40" s="112"/>
-      <c r="L40" s="112"/>
-      <c r="M40" s="112"/>
-      <c r="N40" s="112"/>
-      <c r="O40" s="112"/>
-      <c r="P40" s="112"/>
-      <c r="Q40" s="112"/>
-      <c r="R40" s="112"/>
-      <c r="S40" s="112"/>
-      <c r="T40" s="112"/>
-      <c r="U40" s="112"/>
-      <c r="V40" s="112"/>
-      <c r="W40" s="112"/>
-      <c r="X40" s="112"/>
-      <c r="Y40" s="112"/>
-      <c r="Z40" s="112"/>
-      <c r="AA40" s="112"/>
-      <c r="AB40" s="112"/>
-      <c r="AC40" s="112"/>
-      <c r="AD40" s="112"/>
-      <c r="AE40" s="112"/>
-      <c r="AF40" s="112"/>
-      <c r="AG40" s="112"/>
-      <c r="AH40" s="112"/>
-      <c r="AI40" s="112"/>
-      <c r="AJ40" s="112"/>
-      <c r="AK40" s="112"/>
-      <c r="AL40" s="112"/>
-      <c r="AM40" s="112"/>
-      <c r="AN40" s="112"/>
-      <c r="AO40" s="112"/>
-      <c r="AP40" s="112"/>
-      <c r="AQ40" s="112"/>
-      <c r="AR40" s="112"/>
-      <c r="AS40" s="112"/>
-      <c r="AT40" s="112"/>
-      <c r="AU40" s="112"/>
-      <c r="AV40" s="112"/>
-      <c r="AW40" s="112"/>
-      <c r="AX40" s="112"/>
-      <c r="AY40" s="112"/>
-      <c r="AZ40" s="112"/>
-      <c r="BA40" s="112"/>
-      <c r="BB40" s="112"/>
-      <c r="BC40" s="112"/>
-      <c r="BD40" s="112"/>
-      <c r="BE40" s="112"/>
-      <c r="BF40" s="112"/>
-      <c r="BG40" s="112"/>
-      <c r="BH40" s="112"/>
-      <c r="BI40" s="112"/>
-      <c r="BJ40" s="112"/>
-      <c r="BK40" s="112"/>
-      <c r="BL40" s="112"/>
-      <c r="BM40" s="112"/>
-      <c r="BN40" s="112"/>
-      <c r="BO40" s="112"/>
-      <c r="BP40" s="112"/>
-      <c r="BQ40" s="112"/>
-      <c r="BR40" s="112"/>
-      <c r="BS40" s="112"/>
-      <c r="BT40" s="112"/>
-      <c r="BU40" s="112"/>
-      <c r="BV40" s="112"/>
-      <c r="BW40" s="112"/>
-      <c r="BX40" s="112"/>
-      <c r="BY40" s="112"/>
-      <c r="BZ40" s="112"/>
-      <c r="CA40" s="112"/>
-      <c r="CB40" s="112"/>
-      <c r="CC40" s="112"/>
-      <c r="CD40" s="112"/>
-      <c r="CE40" s="112"/>
-      <c r="CF40" s="112"/>
-      <c r="CG40" s="112"/>
-      <c r="CH40" s="112"/>
-      <c r="CI40" s="112"/>
-      <c r="CJ40" s="112"/>
-      <c r="CK40" s="112"/>
-      <c r="CL40" s="112"/>
-      <c r="CM40" s="112"/>
-      <c r="CN40" s="112"/>
-      <c r="CO40" s="112"/>
-      <c r="CP40" s="112"/>
-      <c r="CQ40" s="112"/>
-      <c r="CR40" s="112"/>
-      <c r="CS40" s="112"/>
-      <c r="CT40" s="112"/>
-      <c r="CU40" s="112"/>
-      <c r="CV40" s="112"/>
-      <c r="CW40" s="113"/>
+      <c r="B40" s="113"/>
+      <c r="C40" s="113"/>
+      <c r="D40" s="113"/>
+      <c r="E40" s="113"/>
+      <c r="F40" s="113"/>
+      <c r="G40" s="113"/>
+      <c r="H40" s="113"/>
+      <c r="I40" s="113"/>
+      <c r="J40" s="113"/>
+      <c r="K40" s="113"/>
+      <c r="L40" s="113"/>
+      <c r="M40" s="113"/>
+      <c r="N40" s="113"/>
+      <c r="O40" s="113"/>
+      <c r="P40" s="113"/>
+      <c r="Q40" s="113"/>
+      <c r="R40" s="113"/>
+      <c r="S40" s="113"/>
+      <c r="T40" s="113"/>
+      <c r="U40" s="113"/>
+      <c r="V40" s="113"/>
+      <c r="W40" s="113"/>
+      <c r="X40" s="113"/>
+      <c r="Y40" s="113"/>
+      <c r="Z40" s="113"/>
+      <c r="AA40" s="113"/>
+      <c r="AB40" s="113"/>
+      <c r="AC40" s="113"/>
+      <c r="AD40" s="113"/>
+      <c r="AE40" s="113"/>
+      <c r="AF40" s="113"/>
+      <c r="AG40" s="113"/>
+      <c r="AH40" s="113"/>
+      <c r="AI40" s="113"/>
+      <c r="AJ40" s="113"/>
+      <c r="AK40" s="113"/>
+      <c r="AL40" s="113"/>
+      <c r="AM40" s="113"/>
+      <c r="AN40" s="113"/>
+      <c r="AO40" s="113"/>
+      <c r="AP40" s="113"/>
+      <c r="AQ40" s="113"/>
+      <c r="AR40" s="113"/>
+      <c r="AS40" s="113"/>
+      <c r="AT40" s="113"/>
+      <c r="AU40" s="113"/>
+      <c r="AV40" s="113"/>
+      <c r="AW40" s="113"/>
+      <c r="AX40" s="113"/>
+      <c r="AY40" s="113"/>
+      <c r="AZ40" s="113"/>
+      <c r="BA40" s="113"/>
+      <c r="BB40" s="113"/>
+      <c r="BC40" s="113"/>
+      <c r="BD40" s="113"/>
+      <c r="BE40" s="113"/>
+      <c r="BF40" s="113"/>
+      <c r="BG40" s="113"/>
+      <c r="BH40" s="113"/>
+      <c r="BI40" s="113"/>
+      <c r="BJ40" s="113"/>
+      <c r="BK40" s="113"/>
+      <c r="BL40" s="113"/>
+      <c r="BM40" s="113"/>
+      <c r="BN40" s="113"/>
+      <c r="BO40" s="113"/>
+      <c r="BP40" s="113"/>
+      <c r="BQ40" s="113"/>
+      <c r="BR40" s="113"/>
+      <c r="BS40" s="113"/>
+      <c r="BT40" s="113"/>
+      <c r="BU40" s="113"/>
+      <c r="BV40" s="113"/>
+      <c r="BW40" s="113"/>
+      <c r="BX40" s="113"/>
+      <c r="BY40" s="113"/>
+      <c r="BZ40" s="113"/>
+      <c r="CA40" s="113"/>
+      <c r="CB40" s="113"/>
+      <c r="CC40" s="113"/>
+      <c r="CD40" s="113"/>
+      <c r="CE40" s="113"/>
+      <c r="CF40" s="113"/>
+      <c r="CG40" s="113"/>
+      <c r="CH40" s="113"/>
+      <c r="CI40" s="113"/>
+      <c r="CJ40" s="113"/>
+      <c r="CK40" s="113"/>
+      <c r="CL40" s="113"/>
+      <c r="CM40" s="113"/>
+      <c r="CN40" s="113"/>
+      <c r="CO40" s="113"/>
+      <c r="CP40" s="113"/>
+      <c r="CQ40" s="113"/>
+      <c r="CR40" s="113"/>
+      <c r="CS40" s="113"/>
+      <c r="CT40" s="113"/>
+      <c r="CU40" s="113"/>
+      <c r="CV40" s="113"/>
+      <c r="CW40" s="114"/>
     </row>
     <row r="41" spans="1:101" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="62" t="s">
@@ -44404,110 +44501,110 @@
         <v>413</v>
       </c>
     </row>
-    <row r="45" spans="1:101" s="111" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="111" t="s">
+    <row r="45" spans="1:101" s="112" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="112" t="s">
         <v>3192</v>
       </c>
-      <c r="B45" s="112"/>
-      <c r="C45" s="112"/>
-      <c r="D45" s="112"/>
-      <c r="E45" s="112"/>
-      <c r="F45" s="112"/>
-      <c r="G45" s="112"/>
-      <c r="H45" s="112"/>
-      <c r="I45" s="112"/>
-      <c r="J45" s="112"/>
-      <c r="K45" s="112"/>
-      <c r="L45" s="112"/>
-      <c r="M45" s="112"/>
-      <c r="N45" s="112"/>
-      <c r="O45" s="112"/>
-      <c r="P45" s="112"/>
-      <c r="Q45" s="112"/>
-      <c r="R45" s="112"/>
-      <c r="S45" s="112"/>
-      <c r="T45" s="112"/>
-      <c r="U45" s="112"/>
-      <c r="V45" s="112"/>
-      <c r="W45" s="112"/>
-      <c r="X45" s="112"/>
-      <c r="Y45" s="112"/>
-      <c r="Z45" s="112"/>
-      <c r="AA45" s="112"/>
-      <c r="AB45" s="112"/>
-      <c r="AC45" s="112"/>
-      <c r="AD45" s="112"/>
-      <c r="AE45" s="112"/>
-      <c r="AF45" s="112"/>
-      <c r="AG45" s="112"/>
-      <c r="AH45" s="112"/>
-      <c r="AI45" s="112"/>
-      <c r="AJ45" s="112"/>
-      <c r="AK45" s="112"/>
-      <c r="AL45" s="112"/>
-      <c r="AM45" s="112"/>
-      <c r="AN45" s="112"/>
-      <c r="AO45" s="112"/>
-      <c r="AP45" s="112"/>
-      <c r="AQ45" s="112"/>
-      <c r="AR45" s="112"/>
-      <c r="AS45" s="112"/>
-      <c r="AT45" s="112"/>
-      <c r="AU45" s="112"/>
-      <c r="AV45" s="112"/>
-      <c r="AW45" s="112"/>
-      <c r="AX45" s="112"/>
-      <c r="AY45" s="112"/>
-      <c r="AZ45" s="112"/>
-      <c r="BA45" s="112"/>
-      <c r="BB45" s="112"/>
-      <c r="BC45" s="112"/>
-      <c r="BD45" s="112"/>
-      <c r="BE45" s="112"/>
-      <c r="BF45" s="112"/>
-      <c r="BG45" s="112"/>
-      <c r="BH45" s="112"/>
-      <c r="BI45" s="112"/>
-      <c r="BJ45" s="112"/>
-      <c r="BK45" s="112"/>
-      <c r="BL45" s="112"/>
-      <c r="BM45" s="112"/>
-      <c r="BN45" s="112"/>
-      <c r="BO45" s="112"/>
-      <c r="BP45" s="112"/>
-      <c r="BQ45" s="112"/>
-      <c r="BR45" s="112"/>
-      <c r="BS45" s="112"/>
-      <c r="BT45" s="112"/>
-      <c r="BU45" s="112"/>
-      <c r="BV45" s="112"/>
-      <c r="BW45" s="112"/>
-      <c r="BX45" s="112"/>
-      <c r="BY45" s="112"/>
-      <c r="BZ45" s="112"/>
-      <c r="CA45" s="112"/>
-      <c r="CB45" s="112"/>
-      <c r="CC45" s="112"/>
-      <c r="CD45" s="112"/>
-      <c r="CE45" s="112"/>
-      <c r="CF45" s="112"/>
-      <c r="CG45" s="112"/>
-      <c r="CH45" s="112"/>
-      <c r="CI45" s="112"/>
-      <c r="CJ45" s="112"/>
-      <c r="CK45" s="112"/>
-      <c r="CL45" s="112"/>
-      <c r="CM45" s="112"/>
-      <c r="CN45" s="112"/>
-      <c r="CO45" s="112"/>
-      <c r="CP45" s="112"/>
-      <c r="CQ45" s="112"/>
-      <c r="CR45" s="112"/>
-      <c r="CS45" s="112"/>
-      <c r="CT45" s="112"/>
-      <c r="CU45" s="112"/>
-      <c r="CV45" s="112"/>
-      <c r="CW45" s="112"/>
+      <c r="B45" s="113"/>
+      <c r="C45" s="113"/>
+      <c r="D45" s="113"/>
+      <c r="E45" s="113"/>
+      <c r="F45" s="113"/>
+      <c r="G45" s="113"/>
+      <c r="H45" s="113"/>
+      <c r="I45" s="113"/>
+      <c r="J45" s="113"/>
+      <c r="K45" s="113"/>
+      <c r="L45" s="113"/>
+      <c r="M45" s="113"/>
+      <c r="N45" s="113"/>
+      <c r="O45" s="113"/>
+      <c r="P45" s="113"/>
+      <c r="Q45" s="113"/>
+      <c r="R45" s="113"/>
+      <c r="S45" s="113"/>
+      <c r="T45" s="113"/>
+      <c r="U45" s="113"/>
+      <c r="V45" s="113"/>
+      <c r="W45" s="113"/>
+      <c r="X45" s="113"/>
+      <c r="Y45" s="113"/>
+      <c r="Z45" s="113"/>
+      <c r="AA45" s="113"/>
+      <c r="AB45" s="113"/>
+      <c r="AC45" s="113"/>
+      <c r="AD45" s="113"/>
+      <c r="AE45" s="113"/>
+      <c r="AF45" s="113"/>
+      <c r="AG45" s="113"/>
+      <c r="AH45" s="113"/>
+      <c r="AI45" s="113"/>
+      <c r="AJ45" s="113"/>
+      <c r="AK45" s="113"/>
+      <c r="AL45" s="113"/>
+      <c r="AM45" s="113"/>
+      <c r="AN45" s="113"/>
+      <c r="AO45" s="113"/>
+      <c r="AP45" s="113"/>
+      <c r="AQ45" s="113"/>
+      <c r="AR45" s="113"/>
+      <c r="AS45" s="113"/>
+      <c r="AT45" s="113"/>
+      <c r="AU45" s="113"/>
+      <c r="AV45" s="113"/>
+      <c r="AW45" s="113"/>
+      <c r="AX45" s="113"/>
+      <c r="AY45" s="113"/>
+      <c r="AZ45" s="113"/>
+      <c r="BA45" s="113"/>
+      <c r="BB45" s="113"/>
+      <c r="BC45" s="113"/>
+      <c r="BD45" s="113"/>
+      <c r="BE45" s="113"/>
+      <c r="BF45" s="113"/>
+      <c r="BG45" s="113"/>
+      <c r="BH45" s="113"/>
+      <c r="BI45" s="113"/>
+      <c r="BJ45" s="113"/>
+      <c r="BK45" s="113"/>
+      <c r="BL45" s="113"/>
+      <c r="BM45" s="113"/>
+      <c r="BN45" s="113"/>
+      <c r="BO45" s="113"/>
+      <c r="BP45" s="113"/>
+      <c r="BQ45" s="113"/>
+      <c r="BR45" s="113"/>
+      <c r="BS45" s="113"/>
+      <c r="BT45" s="113"/>
+      <c r="BU45" s="113"/>
+      <c r="BV45" s="113"/>
+      <c r="BW45" s="113"/>
+      <c r="BX45" s="113"/>
+      <c r="BY45" s="113"/>
+      <c r="BZ45" s="113"/>
+      <c r="CA45" s="113"/>
+      <c r="CB45" s="113"/>
+      <c r="CC45" s="113"/>
+      <c r="CD45" s="113"/>
+      <c r="CE45" s="113"/>
+      <c r="CF45" s="113"/>
+      <c r="CG45" s="113"/>
+      <c r="CH45" s="113"/>
+      <c r="CI45" s="113"/>
+      <c r="CJ45" s="113"/>
+      <c r="CK45" s="113"/>
+      <c r="CL45" s="113"/>
+      <c r="CM45" s="113"/>
+      <c r="CN45" s="113"/>
+      <c r="CO45" s="113"/>
+      <c r="CP45" s="113"/>
+      <c r="CQ45" s="113"/>
+      <c r="CR45" s="113"/>
+      <c r="CS45" s="113"/>
+      <c r="CT45" s="113"/>
+      <c r="CU45" s="113"/>
+      <c r="CV45" s="113"/>
+      <c r="CW45" s="113"/>
     </row>
     <row r="46" spans="1:101" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="58" t="s">
@@ -44975,16 +45072,16 @@
       </c>
     </row>
     <row r="60" spans="1:101" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="115" t="s">
+      <c r="A60" s="116" t="s">
         <v>188</v>
       </c>
-      <c r="B60" s="115" t="s">
+      <c r="B60" s="116" t="s">
         <v>3382</v>
       </c>
     </row>
     <row r="61" spans="1:101" x14ac:dyDescent="0.25">
-      <c r="A61" s="116"/>
-      <c r="B61" s="116"/>
+      <c r="A61" s="117"/>
+      <c r="B61" s="117"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -45369,10 +45466,10 @@
       <c r="A8" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="B8" s="117" t="s">
+      <c r="B8" s="118" t="s">
         <v>3383</v>
       </c>
-      <c r="C8" s="117"/>
+      <c r="C8" s="118"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -45389,7 +45486,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D8" sqref="D8"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45419,8 +45516,16 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>3496</v>
+      </c>
+    </row>
     <row r="4" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -45478,8 +45583,8 @@
         <v>2559</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="110" t="s">
+    <row r="14" spans="1:6" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="111" t="s">
         <v>3195</v>
       </c>
     </row>
@@ -45788,8 +45893,8 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="110" t="s">
+    <row r="32" spans="1:6" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="111" t="s">
         <v>3191</v>
       </c>
     </row>
@@ -45874,8 +45979,8 @@
         <v>340</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="110" t="s">
+    <row r="37" spans="1:6" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="111" t="s">
         <v>3192</v>
       </c>
     </row>
@@ -46169,7 +46274,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B12" sqref="B12"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46200,8 +46305,16 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>3496</v>
+      </c>
+    </row>
     <row r="4" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:6" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -46255,8 +46368,8 @@
         <v>2558</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="110" t="s">
+    <row r="14" spans="1:6" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="111" t="s">
         <v>3195</v>
       </c>
     </row>
@@ -46384,8 +46497,8 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:6" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="110" t="s">
+    <row r="22" spans="1:6" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="111" t="s">
         <v>3192</v>
       </c>
     </row>
@@ -46610,7 +46723,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:XFD10"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46637,8 +46750,16 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>3496</v>
+      </c>
+    </row>
     <row r="4" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -46734,7 +46855,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" sqref="A1:XFD10"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46779,8 +46900,16 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>3496</v>
+      </c>
+    </row>
     <row r="4" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:10" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -46963,7 +47092,7 @@
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A34" sqref="A34"/>
-      <selection pane="topRight" sqref="A1:XFD10"/>
+      <selection pane="topRight" activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -46991,8 +47120,16 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="19" t="s">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>3496</v>
+      </c>
+    </row>
     <row r="4" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="6" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -47000,8 +47137,8 @@
     <row r="8" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:5" s="19" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="110" t="s">
+    <row r="11" spans="1:5" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="111" t="s">
         <v>3196</v>
       </c>
     </row>
@@ -47028,8 +47165,8 @@
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="110" t="s">
+    <row r="16" spans="1:5" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="111" t="s">
         <v>3197</v>
       </c>
     </row>
@@ -47123,8 +47260,8 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:2" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="110" t="s">
+    <row r="29" spans="1:2" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="111" t="s">
         <v>3198</v>
       </c>
     </row>
@@ -47250,8 +47387,8 @@
         <v>161</v>
       </c>
     </row>
-    <row r="49" spans="1:2" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="110" t="s">
+    <row r="49" spans="1:2" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="111" t="s">
         <v>3199</v>
       </c>
     </row>
@@ -47293,8 +47430,8 @@
         <v>2425</v>
       </c>
     </row>
-    <row r="55" spans="1:2" s="110" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="110" t="s">
+    <row r="55" spans="1:2" s="111" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="111" t="s">
         <v>3200</v>
       </c>
     </row>

</xml_diff>